<commit_message>
Keep Version 0.91 Commit
Refer to changelog.  Weapons should now be fixed among other things with various enemy precaches.
</commit_message>
<xml_diff>
--- a/KeepFeatureChecklist.xlsx
+++ b/KeepFeatureChecklist.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5970" windowHeight="1035" tabRatio="724"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="5970" windowHeight="1035" tabRatio="724" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Enemies" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Brush Entities'!$A$1:$L$60</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Enemies!$A$2:$N$145</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Full List Per Mod'!$A$1:$B$409</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Items!$A$2:$L$206</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Items!$A$2:$L$207</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Point Entities'!$A$2:$L$135</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Traps!$A$2:$L$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Weapons!$A$2:$L$2</definedName>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2539" uniqueCount="1021">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2543" uniqueCount="1023">
   <si>
     <t>KEEP - ENEMIES TO INCLUDE</t>
   </si>
@@ -3107,13 +3107,19 @@
   </si>
   <si>
     <t>Sheep (DENIZEN)</t>
+  </si>
+  <si>
+    <t>Health Vial</t>
+  </si>
+  <si>
+    <t>item_healthvial</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3130,6 +3136,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3201,7 +3214,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -3233,6 +3246,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3515,9 +3529,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N716"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F112" sqref="F112"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3615,7 +3629,7 @@
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
+      <c r="E4" s="7"/>
       <c r="F4" s="5" t="s">
         <v>742</v>
       </c>
@@ -3641,7 +3655,7 @@
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
+      <c r="E5" s="7"/>
       <c r="F5" s="5" t="s">
         <v>744</v>
       </c>
@@ -3791,7 +3805,7 @@
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
+      <c r="E11" s="7"/>
       <c r="F11" s="5" t="s">
         <v>989</v>
       </c>
@@ -3821,7 +3835,7 @@
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
+      <c r="E12" s="7"/>
       <c r="F12" s="5" t="s">
         <v>688</v>
       </c>
@@ -3869,7 +3883,7 @@
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="6"/>
-      <c r="E14" s="5"/>
+      <c r="E14" s="7"/>
       <c r="F14" s="5" t="s">
         <v>799</v>
       </c>
@@ -3895,7 +3909,7 @@
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
-      <c r="E15" s="5"/>
+      <c r="E15" s="7"/>
       <c r="F15" s="5" t="s">
         <v>955</v>
       </c>
@@ -3917,7 +3931,7 @@
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="6"/>
-      <c r="E16" s="5"/>
+      <c r="E16" s="7"/>
       <c r="F16" s="5" t="s">
         <v>793</v>
       </c>
@@ -4276,7 +4290,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
-      <c r="B31" s="6"/>
+      <c r="B31" s="19"/>
       <c r="C31" s="7"/>
       <c r="D31" s="6"/>
       <c r="E31" s="7"/>
@@ -4350,7 +4364,7 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
-      <c r="B34" s="6"/>
+      <c r="B34" s="7"/>
       <c r="C34" s="7"/>
       <c r="D34" s="6"/>
       <c r="E34" s="7"/>
@@ -4526,7 +4540,7 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
-      <c r="B41" s="6"/>
+      <c r="B41" s="7"/>
       <c r="C41" s="7"/>
       <c r="D41" s="6"/>
       <c r="E41" s="7"/>
@@ -4576,7 +4590,7 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
-      <c r="B43" s="6"/>
+      <c r="B43" s="7"/>
       <c r="C43" s="7"/>
       <c r="D43" s="6"/>
       <c r="E43" s="7"/>
@@ -4874,7 +4888,7 @@
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="7"/>
-      <c r="B55" s="6"/>
+      <c r="B55" s="7"/>
       <c r="C55" s="7"/>
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
@@ -4902,10 +4916,10 @@
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="7"/>
-      <c r="B56" s="5"/>
+      <c r="B56" s="7"/>
       <c r="C56" s="7"/>
       <c r="D56" s="6"/>
-      <c r="E56" s="5"/>
+      <c r="E56" s="7"/>
       <c r="F56" s="5" t="s">
         <v>800</v>
       </c>
@@ -4976,7 +4990,7 @@
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="7"/>
-      <c r="B59" s="6"/>
+      <c r="B59" s="7"/>
       <c r="C59" s="7"/>
       <c r="D59" s="6"/>
       <c r="E59" s="6"/>
@@ -5260,7 +5274,7 @@
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="7"/>
-      <c r="B70" s="6"/>
+      <c r="B70" s="7"/>
       <c r="C70" s="7"/>
       <c r="D70" s="6"/>
       <c r="E70" s="6"/>
@@ -5394,7 +5408,7 @@
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="7"/>
-      <c r="B75" s="6"/>
+      <c r="B75" s="7"/>
       <c r="C75" s="7"/>
       <c r="D75" s="6"/>
       <c r="E75" s="6"/>
@@ -5442,7 +5456,7 @@
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="7"/>
-      <c r="B77" s="6"/>
+      <c r="B77" s="7"/>
       <c r="C77" s="7"/>
       <c r="D77" s="6"/>
       <c r="E77" s="6"/>
@@ -5742,7 +5756,7 @@
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" s="7"/>
-      <c r="B89" s="6"/>
+      <c r="B89" s="7"/>
       <c r="C89" s="7"/>
       <c r="D89" s="6"/>
       <c r="E89" s="6"/>
@@ -6414,7 +6428,7 @@
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A115" s="7"/>
-      <c r="B115" s="6"/>
+      <c r="B115" s="7"/>
       <c r="C115" s="7"/>
       <c r="D115" s="6"/>
       <c r="E115" s="6"/>
@@ -6442,7 +6456,7 @@
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A116" s="7"/>
-      <c r="B116" s="5"/>
+      <c r="B116" s="7"/>
       <c r="C116" s="7"/>
       <c r="D116" s="6"/>
       <c r="E116" s="5"/>
@@ -16234,7 +16248,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16402,7 +16416,7 @@
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
-      <c r="D8" s="6"/>
+      <c r="D8" s="7"/>
       <c r="E8" s="5" t="s">
         <v>940</v>
       </c>
@@ -16426,7 +16440,7 @@
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
-      <c r="D9" s="6"/>
+      <c r="D9" s="7"/>
       <c r="E9" s="5" t="s">
         <v>951</v>
       </c>
@@ -16450,7 +16464,7 @@
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
-      <c r="D10" s="6"/>
+      <c r="D10" s="7"/>
       <c r="E10" s="5" t="s">
         <v>941</v>
       </c>
@@ -16560,7 +16574,7 @@
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
-      <c r="D15" s="6"/>
+      <c r="D15" s="7"/>
       <c r="E15" s="5" t="s">
         <v>944</v>
       </c>
@@ -16712,7 +16726,7 @@
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
-      <c r="D22" s="6"/>
+      <c r="D22" s="7"/>
       <c r="E22" s="5" t="s">
         <v>946</v>
       </c>
@@ -16758,7 +16772,7 @@
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
-      <c r="D24" s="6"/>
+      <c r="D24" s="7"/>
       <c r="E24" s="5" t="s">
         <v>954</v>
       </c>
@@ -16782,7 +16796,7 @@
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
-      <c r="D25" s="6"/>
+      <c r="D25" s="7"/>
       <c r="E25" s="5" t="s">
         <v>948</v>
       </c>
@@ -16932,7 +16946,7 @@
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
-      <c r="D32" s="6"/>
+      <c r="D32" s="7"/>
       <c r="E32" s="5" t="s">
         <v>950</v>
       </c>
@@ -16996,7 +17010,7 @@
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
-      <c r="D35" s="6"/>
+      <c r="D35" s="7"/>
       <c r="E35" s="5" t="s">
         <v>772</v>
       </c>
@@ -17018,7 +17032,7 @@
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
-      <c r="D36" s="6"/>
+      <c r="D36" s="7"/>
       <c r="E36" s="5" t="s">
         <v>850</v>
       </c>
@@ -17040,7 +17054,7 @@
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
-      <c r="D37" s="6"/>
+      <c r="D37" s="7"/>
       <c r="E37" s="5" t="s">
         <v>770</v>
       </c>
@@ -17060,7 +17074,7 @@
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="7"/>
-      <c r="D38" s="6"/>
+      <c r="D38" s="7"/>
       <c r="E38" s="5" t="s">
         <v>769</v>
       </c>
@@ -17104,7 +17118,7 @@
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
-      <c r="D40" s="6"/>
+      <c r="D40" s="7"/>
       <c r="E40" s="5" t="s">
         <v>859</v>
       </c>
@@ -17124,7 +17138,7 @@
       <c r="A41" s="7"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
-      <c r="D41" s="6"/>
+      <c r="D41" s="7"/>
       <c r="E41" s="5" t="s">
         <v>860</v>
       </c>
@@ -25993,11 +26007,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L670"/>
+  <dimension ref="A1:L671"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26079,7 +26093,7 @@
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
-      <c r="D4" s="6"/>
+      <c r="D4" s="7"/>
       <c r="E4" s="5" t="s">
         <v>181</v>
       </c>
@@ -26099,7 +26113,7 @@
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
-      <c r="D5" s="6"/>
+      <c r="D5" s="7"/>
       <c r="E5" s="5" t="s">
         <v>180</v>
       </c>
@@ -26139,7 +26153,7 @@
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
-      <c r="D7" s="6"/>
+      <c r="D7" s="7"/>
       <c r="E7" s="5" t="s">
         <v>179</v>
       </c>
@@ -26823,7 +26837,7 @@
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
-      <c r="D40" s="6"/>
+      <c r="D40" s="7"/>
       <c r="E40" s="5" t="s">
         <v>189</v>
       </c>
@@ -26846,22 +26860,24 @@
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="7"/>
       <c r="E41" s="5" t="s">
-        <v>163</v>
+        <v>1021</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>161</v>
+        <v>1022</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
-      <c r="L41" s="5"/>
+      <c r="L41" s="5" t="s">
+        <v>1006</v>
+      </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
@@ -26869,10 +26885,10 @@
       <c r="C42" s="7"/>
       <c r="D42" s="6"/>
       <c r="E42" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G42" s="4" t="s">
         <v>61</v>
@@ -26885,17 +26901,17 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
-      <c r="B43" s="13"/>
+      <c r="B43" s="7"/>
       <c r="C43" s="7"/>
       <c r="D43" s="6"/>
       <c r="E43" s="5" t="s">
-        <v>193</v>
+        <v>164</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>192</v>
+        <v>162</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H43" s="4"/>
       <c r="I43" s="4"/>
@@ -26905,17 +26921,17 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
-      <c r="B44" s="7"/>
+      <c r="B44" s="13"/>
       <c r="C44" s="7"/>
       <c r="D44" s="6"/>
       <c r="E44" s="5" t="s">
-        <v>398</v>
+        <v>193</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>394</v>
+        <v>192</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
@@ -26929,10 +26945,10 @@
       <c r="C45" s="7"/>
       <c r="D45" s="6"/>
       <c r="E45" s="5" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G45" s="4" t="s">
         <v>62</v>
@@ -26949,23 +26965,19 @@
       <c r="C46" s="7"/>
       <c r="D46" s="6"/>
       <c r="E46" s="5" t="s">
-        <v>125</v>
+        <v>399</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>190</v>
+        <v>395</v>
       </c>
       <c r="G46" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="H46" s="4" t="s">
-        <v>63</v>
-      </c>
+      <c r="H46" s="4"/>
       <c r="I46" s="4"/>
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
-      <c r="L46" s="5" t="s">
-        <v>191</v>
-      </c>
+      <c r="L46" s="5"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
@@ -26973,19 +26985,23 @@
       <c r="C47" s="7"/>
       <c r="D47" s="6"/>
       <c r="E47" s="5" t="s">
-        <v>211</v>
+        <v>125</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>602</v>
+        <v>190</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="H47" s="4"/>
+        <v>62</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="I47" s="4"/>
       <c r="J47" s="4"/>
       <c r="K47" s="4"/>
-      <c r="L47" s="5"/>
+      <c r="L47" s="5" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
@@ -26993,13 +27009,13 @@
       <c r="C48" s="7"/>
       <c r="D48" s="6"/>
       <c r="E48" s="5" t="s">
-        <v>400</v>
+        <v>211</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>396</v>
+        <v>602</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>62</v>
+        <v>208</v>
       </c>
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
@@ -27013,10 +27029,10 @@
       <c r="C49" s="7"/>
       <c r="D49" s="6"/>
       <c r="E49" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="G49" s="4" t="s">
         <v>62</v>
@@ -27033,21 +27049,19 @@
       <c r="C50" s="7"/>
       <c r="D50" s="6"/>
       <c r="E50" s="5" t="s">
-        <v>720</v>
+        <v>401</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>707</v>
+        <v>397</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>694</v>
+        <v>62</v>
       </c>
       <c r="H50" s="4"/>
       <c r="I50" s="4"/>
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
-      <c r="L50" s="5" t="s">
-        <v>1015</v>
-      </c>
+      <c r="L50" s="5"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
@@ -27055,19 +27069,21 @@
       <c r="C51" s="7"/>
       <c r="D51" s="6"/>
       <c r="E51" s="5" t="s">
-        <v>156</v>
+        <v>720</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>186</v>
+        <v>707</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>61</v>
+        <v>694</v>
       </c>
       <c r="H51" s="4"/>
       <c r="I51" s="4"/>
       <c r="J51" s="4"/>
       <c r="K51" s="4"/>
-      <c r="L51" s="5"/>
+      <c r="L51" s="5" t="s">
+        <v>1015</v>
+      </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="7"/>
@@ -27075,10 +27091,10 @@
       <c r="C52" s="7"/>
       <c r="D52" s="6"/>
       <c r="E52" s="5" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="G52" s="4" t="s">
         <v>61</v>
@@ -27095,10 +27111,10 @@
       <c r="C53" s="7"/>
       <c r="D53" s="6"/>
       <c r="E53" s="5" t="s">
-        <v>183</v>
+        <v>154</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="G53" s="4" t="s">
         <v>61</v>
@@ -27115,13 +27131,13 @@
       <c r="C54" s="7"/>
       <c r="D54" s="6"/>
       <c r="E54" s="5" t="s">
-        <v>710</v>
+        <v>183</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>708</v>
+        <v>182</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>694</v>
+        <v>61</v>
       </c>
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
@@ -27135,13 +27151,13 @@
       <c r="C55" s="7"/>
       <c r="D55" s="6"/>
       <c r="E55" s="5" t="s">
-        <v>155</v>
+        <v>710</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>185</v>
+        <v>708</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>61</v>
+        <v>694</v>
       </c>
       <c r="H55" s="4"/>
       <c r="I55" s="4"/>
@@ -27155,17 +27171,15 @@
       <c r="C56" s="7"/>
       <c r="D56" s="6"/>
       <c r="E56" s="5" t="s">
-        <v>613</v>
+        <v>155</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>706</v>
+        <v>185</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>694</v>
-      </c>
-      <c r="H56" s="4" t="s">
-        <v>65</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="H56" s="4"/>
       <c r="I56" s="4"/>
       <c r="J56" s="4"/>
       <c r="K56" s="4"/>
@@ -27173,45 +27187,47 @@
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
-      <c r="B57" s="6"/>
+      <c r="B57" s="7"/>
       <c r="C57" s="7"/>
       <c r="D57" s="6"/>
       <c r="E57" s="5" t="s">
-        <v>196</v>
+        <v>613</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>195</v>
+        <v>706</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="H57" s="4"/>
+        <v>694</v>
+      </c>
+      <c r="H57" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="I57" s="4"/>
       <c r="J57" s="4"/>
       <c r="K57" s="4"/>
-      <c r="L57" s="5" t="s">
-        <v>1016</v>
-      </c>
+      <c r="L57" s="5"/>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="7"/>
-      <c r="B58" s="7"/>
+      <c r="B58" s="6"/>
       <c r="C58" s="7"/>
       <c r="D58" s="6"/>
       <c r="E58" s="5" t="s">
-        <v>721</v>
+        <v>196</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>709</v>
+        <v>195</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>694</v>
+        <v>63</v>
       </c>
       <c r="H58" s="4"/>
       <c r="I58" s="4"/>
       <c r="J58" s="4"/>
       <c r="K58" s="4"/>
-      <c r="L58" s="5"/>
+      <c r="L58" s="5" t="s">
+        <v>1016</v>
+      </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="7"/>
@@ -27222,7 +27238,7 @@
         <v>721</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>911</v>
+        <v>709</v>
       </c>
       <c r="G59" s="4" t="s">
         <v>694</v>
@@ -27242,7 +27258,7 @@
         <v>721</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="G60" s="4" t="s">
         <v>694</v>
@@ -27254,13 +27270,19 @@
       <c r="L60" s="5"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A61" s="5"/>
-      <c r="B61" s="5"/>
-      <c r="C61" s="5"/>
+      <c r="A61" s="7"/>
+      <c r="B61" s="7"/>
+      <c r="C61" s="7"/>
       <c r="D61" s="6"/>
-      <c r="E61" s="5"/>
-      <c r="F61" s="5"/>
-      <c r="G61" s="4"/>
+      <c r="E61" s="5" t="s">
+        <v>721</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>912</v>
+      </c>
+      <c r="G61" s="4" t="s">
+        <v>694</v>
+      </c>
       <c r="H61" s="4"/>
       <c r="I61" s="4"/>
       <c r="J61" s="4"/>
@@ -27453,7 +27475,7 @@
       <c r="A75" s="5"/>
       <c r="B75" s="5"/>
       <c r="C75" s="5"/>
-      <c r="D75" s="5"/>
+      <c r="D75" s="6"/>
       <c r="E75" s="5"/>
       <c r="F75" s="5"/>
       <c r="G75" s="4"/>
@@ -35626,6 +35648,9 @@
       <c r="L658" s="5"/>
     </row>
     <row r="659" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A659" s="5"/>
+      <c r="B659" s="5"/>
+      <c r="C659" s="5"/>
       <c r="D659" s="5"/>
       <c r="E659" s="5"/>
       <c r="F659" s="5"/>
@@ -35692,6 +35717,7 @@
       <c r="L664" s="5"/>
     </row>
     <row r="665" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D665" s="5"/>
       <c r="E665" s="5"/>
       <c r="F665" s="5"/>
       <c r="G665" s="4"/>
@@ -35750,6 +35776,16 @@
       <c r="J670" s="4"/>
       <c r="K670" s="4"/>
       <c r="L670" s="5"/>
+    </row>
+    <row r="671" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E671" s="5"/>
+      <c r="F671" s="5"/>
+      <c r="G671" s="4"/>
+      <c r="H671" s="4"/>
+      <c r="I671" s="4"/>
+      <c r="J671" s="4"/>
+      <c r="K671" s="4"/>
+      <c r="L671" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Pre-1.00 Early Alpha to the Alpha
Added new conback to display KEEP and 1.00. Added new AI system. Commonized AI for most monsters except for a handful of bosses. Added shrines. Added more monsters, mostly madfox creations. Added Gyro2.1a physics system.  Added lots of resources from redfield and dwell and copper.
</commit_message>
<xml_diff>
--- a/KeepFeatureChecklist.xlsx
+++ b/KeepFeatureChecklist.xlsx
@@ -19,13 +19,15 @@
     <sheet name="Brush Entities" sheetId="4" r:id="rId5"/>
     <sheet name="Point Entities" sheetId="5" r:id="rId6"/>
     <sheet name="Full List Per Mod" sheetId="8" r:id="rId7"/>
+    <sheet name="Mod Inclusion Checklist" sheetId="9" r:id="rId8"/>
+    <sheet name="Sheet2" sheetId="10" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Brush Entities'!$A$1:$L$60</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Enemies!$A$2:$N$148</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Enemies!$A$2:$N$151</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Full List Per Mod'!$A$1:$B$409</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Items!$A$2:$L$207</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Point Entities'!$A$2:$L$135</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Point Entities'!$A$2:$L$139</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Traps!$A$2:$L$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Weapons!$A$2:$L$2</definedName>
   </definedNames>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2552" uniqueCount="1029">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2658" uniqueCount="1104">
   <si>
     <t>KEEP - ENEMIES TO INCLUDE</t>
   </si>
@@ -3131,13 +3133,238 @@
   </si>
   <si>
     <t>monster_nehahra</t>
+  </si>
+  <si>
+    <t>trigger_enemy</t>
+  </si>
+  <si>
+    <t>Trigger Enemy</t>
+  </si>
+  <si>
+    <t>trigger_victory</t>
+  </si>
+  <si>
+    <t>Trigger Victory</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Partial</t>
+  </si>
+  <si>
+    <t>Hipnotic (Mission Pack 1)</t>
+  </si>
+  <si>
+    <t>KEEP - MODS AND GAMES INCLUDED</t>
+  </si>
+  <si>
+    <t>Mod or Game Name</t>
+  </si>
+  <si>
+    <t>Rogue (Mission Pack 2)</t>
+  </si>
+  <si>
+    <t>Heretic II</t>
+  </si>
+  <si>
+    <t>Kinn (Marcher &amp; Bastion)</t>
+  </si>
+  <si>
+    <t>Not adding more.  Excluded quite a few DarkPlaces specific effects and cvars.</t>
+  </si>
+  <si>
+    <t>extras_r4 &amp; extras_r5</t>
+  </si>
+  <si>
+    <t>Includes khreathor's updates</t>
+  </si>
+  <si>
+    <t>AoA (Arms of Asgaard)</t>
+  </si>
+  <si>
+    <t>Heavily modified by ryanscissorhands specifically for Keep</t>
+  </si>
+  <si>
+    <t>back2forwards</t>
+  </si>
+  <si>
+    <t>monster_hell_pointknight</t>
+  </si>
+  <si>
+    <t>Electrical Death Knight</t>
+  </si>
+  <si>
+    <t>monster_hell_knight</t>
+  </si>
+  <si>
+    <t>monster_hell_knight_enforcer</t>
+  </si>
+  <si>
+    <t>Saber Enforcer</t>
+  </si>
+  <si>
+    <t>Enforcer with a light saber</t>
+  </si>
+  <si>
+    <t>ITS (In The Shadows)</t>
+  </si>
+  <si>
+    <t>Kurok</t>
+  </si>
+  <si>
+    <t>Likely not going to include the stealth mode and amulet.</t>
+  </si>
+  <si>
+    <t>Not adding more.  Quoth 2.2 source not available.</t>
+  </si>
+  <si>
+    <t>The Lieutenant</t>
+  </si>
+  <si>
+    <t>Stuff from the author of lthsp3 and back2forwards</t>
+  </si>
+  <si>
+    <t>Random Community Contributions</t>
+  </si>
+  <si>
+    <t>Madfox</t>
+  </si>
+  <si>
+    <t>Cool stuff from madfox, lots of different enemies and effects.</t>
+  </si>
+  <si>
+    <t>Keep Extras - Not Directly Used by Mod</t>
+  </si>
+  <si>
+    <t>Useful models for decorations and sounds for custom effects.</t>
+  </si>
+  <si>
+    <t>Newhouse</t>
+  </si>
+  <si>
+    <t>OUM (Operation Urth Majik)</t>
+  </si>
+  <si>
+    <t>Don't have swinging gate, fast zombies, prox mines, or specialty angels.</t>
+  </si>
+  <si>
+    <t>Don't have the dispensers/healthpanels, turret incomplete</t>
+  </si>
+  <si>
+    <t>Ravenkeep</t>
+  </si>
+  <si>
+    <t>Lots of great stuff, need to add</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>Rubicon + Rubicon 2 + RRP</t>
+  </si>
+  <si>
+    <t>Need misc_flag, func_turret incomplete.</t>
+  </si>
+  <si>
+    <t>Need to finish adding uber scrag, incomplete.  Need monster_azoth</t>
+  </si>
+  <si>
+    <t>Arcane Dimensions (AD 1.81)</t>
+  </si>
+  <si>
+    <t>Gyro 2 Physics</t>
+  </si>
+  <si>
+    <t>Vigil</t>
+  </si>
+  <si>
+    <t>misc_deadplayer</t>
+  </si>
+  <si>
+    <t>Corpse Player</t>
+  </si>
+  <si>
+    <t>Trigger Congratulations</t>
+  </si>
+  <si>
+    <t>trigger_vigend</t>
+  </si>
+  <si>
+    <t>Drake (Includes SOE, Rapture, Unforgiven, Something Wicked)</t>
+  </si>
+  <si>
+    <t>Twisted Christmas</t>
+  </si>
+  <si>
+    <t>Included in AD.</t>
+  </si>
+  <si>
+    <t>tfl4</t>
+  </si>
+  <si>
+    <t>Rotating object hack.  Included for posterity.</t>
+  </si>
+  <si>
+    <t>tefdbl3</t>
+  </si>
+  <si>
+    <t>Cool black widow spider, aka redback</t>
+  </si>
+  <si>
+    <t>AD Test Map</t>
+  </si>
+  <si>
+    <t>test_trigger_fog</t>
+  </si>
+  <si>
+    <t>test_treleporter</t>
+  </si>
+  <si>
+    <t>test_angletarget</t>
+  </si>
+  <si>
+    <t>test_artifact_blastbelt</t>
+  </si>
+  <si>
+    <t>test_artifact_jboots</t>
+  </si>
+  <si>
+    <t>test_artifact_lavashield</t>
+  </si>
+  <si>
+    <t>test_corpsemodel</t>
+  </si>
+  <si>
+    <t>test_func_breakable_flesh</t>
+  </si>
+  <si>
+    <t>test_func_train</t>
+  </si>
+  <si>
+    <t>test_marshlight</t>
+  </si>
+  <si>
+    <t>test_misc_camera</t>
+  </si>
+  <si>
+    <t>test_misc_gibfountain</t>
+  </si>
+  <si>
+    <t>monster_spellmaster</t>
+  </si>
+  <si>
+    <t>This was in Madfox's Phantom Pholly map</t>
+  </si>
+  <si>
+    <t>Baseboss</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3161,6 +3388,22 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3192,7 +3435,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -3228,11 +3471,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -3265,6 +3545,39 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3545,11 +3858,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N719"/>
+  <dimension ref="A1:N722"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G86" sqref="G86"/>
+      <pane ySplit="2" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E133" sqref="E133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3559,11 +3872,12 @@
     <col min="3" max="3" width="6.7109375" customWidth="1"/>
     <col min="4" max="4" width="6.7109375" style="15" customWidth="1"/>
     <col min="5" max="5" width="10.5703125" customWidth="1"/>
-    <col min="6" max="6" width="23.7109375" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" customWidth="1"/>
     <col min="7" max="7" width="63.5703125" customWidth="1"/>
     <col min="8" max="8" width="9.7109375" customWidth="1"/>
     <col min="9" max="9" width="9.85546875" customWidth="1"/>
-    <col min="10" max="13" width="10.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" style="1" customWidth="1"/>
+    <col min="11" max="13" width="10.28515625" style="1" customWidth="1"/>
     <col min="14" max="14" width="85" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5064,7 +5378,7 @@
         <v>105</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>656</v>
+        <v>1049</v>
       </c>
       <c r="H61" s="5">
         <v>250</v>
@@ -5115,49 +5429,57 @@
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
       <c r="D63" s="6"/>
-      <c r="E63" s="5"/>
+      <c r="E63" s="6"/>
       <c r="F63" s="5" t="s">
-        <v>779</v>
+        <v>1051</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>777</v>
+        <v>1050</v>
       </c>
       <c r="H63" s="5">
-        <v>400</v>
+        <v>105</v>
       </c>
       <c r="I63" s="5"/>
       <c r="J63" s="4" t="s">
-        <v>694</v>
+        <v>1046</v>
       </c>
       <c r="K63" s="4"/>
       <c r="L63" s="4"/>
       <c r="M63" s="4"/>
-      <c r="N63" s="5"/>
+      <c r="N63" s="5" t="s">
+        <v>1052</v>
+      </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="7"/>
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
       <c r="D64" s="6"/>
-      <c r="E64" s="5"/>
+      <c r="E64" s="6"/>
       <c r="F64" s="5" t="s">
-        <v>797</v>
+        <v>1048</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>796</v>
+        <v>1047</v>
       </c>
       <c r="H64" s="5">
-        <v>900</v>
+        <v>250</v>
       </c>
       <c r="I64" s="5"/>
       <c r="J64" s="4" t="s">
-        <v>694</v>
-      </c>
-      <c r="K64" s="4"/>
-      <c r="L64" s="4"/>
-      <c r="M64" s="4"/>
+        <v>61</v>
+      </c>
+      <c r="K64" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="L64" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="M64" s="4" t="s">
+        <v>67</v>
+      </c>
       <c r="N64" s="5" t="s">
-        <v>923</v>
+        <v>116</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.25">
@@ -5165,21 +5487,19 @@
       <c r="B65" s="7"/>
       <c r="C65" s="7"/>
       <c r="D65" s="6"/>
-      <c r="E65" s="6"/>
+      <c r="E65" s="5"/>
       <c r="F65" s="5" t="s">
-        <v>649</v>
+        <v>779</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>52</v>
+        <v>777</v>
       </c>
       <c r="H65" s="5">
-        <v>200</v>
-      </c>
-      <c r="I65" s="5">
-        <v>250</v>
-      </c>
+        <v>400</v>
+      </c>
+      <c r="I65" s="5"/>
       <c r="J65" s="4" t="s">
-        <v>63</v>
+        <v>694</v>
       </c>
       <c r="K65" s="4"/>
       <c r="L65" s="4"/>
@@ -5191,26 +5511,26 @@
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
       <c r="D66" s="6"/>
-      <c r="E66" s="6"/>
+      <c r="E66" s="5"/>
       <c r="F66" s="5" t="s">
-        <v>650</v>
+        <v>797</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>53</v>
+        <v>796</v>
       </c>
       <c r="H66" s="5">
-        <v>300</v>
-      </c>
-      <c r="I66" s="5">
-        <v>350</v>
-      </c>
+        <v>900</v>
+      </c>
+      <c r="I66" s="5"/>
       <c r="J66" s="4" t="s">
-        <v>63</v>
+        <v>694</v>
       </c>
       <c r="K66" s="4"/>
       <c r="L66" s="4"/>
       <c r="M66" s="4"/>
-      <c r="N66" s="5"/>
+      <c r="N66" s="5" t="s">
+        <v>923</v>
+      </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="7"/>
@@ -5219,10 +5539,10 @@
       <c r="D67" s="6"/>
       <c r="E67" s="6"/>
       <c r="F67" s="5" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H67" s="5">
         <v>200</v>
@@ -5245,26 +5565,24 @@
       <c r="D68" s="6"/>
       <c r="E68" s="6"/>
       <c r="F68" s="5" t="s">
-        <v>926</v>
+        <v>650</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>927</v>
-      </c>
-      <c r="H68" s="5"/>
-      <c r="I68" s="5"/>
+        <v>53</v>
+      </c>
+      <c r="H68" s="5">
+        <v>300</v>
+      </c>
+      <c r="I68" s="5">
+        <v>350</v>
+      </c>
       <c r="J68" s="4" t="s">
-        <v>914</v>
-      </c>
-      <c r="K68" s="4" t="s">
-        <v>930</v>
-      </c>
-      <c r="L68" s="4" t="s">
-        <v>928</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="K68" s="4"/>
+      <c r="L68" s="4"/>
       <c r="M68" s="4"/>
-      <c r="N68" s="5" t="s">
-        <v>929</v>
-      </c>
+      <c r="N68" s="5"/>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="7"/>
@@ -5273,15 +5591,17 @@
       <c r="D69" s="6"/>
       <c r="E69" s="6"/>
       <c r="F69" s="5" t="s">
-        <v>674</v>
+        <v>651</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>675</v>
+        <v>54</v>
       </c>
       <c r="H69" s="5">
-        <v>50000</v>
-      </c>
-      <c r="I69" s="5"/>
+        <v>200</v>
+      </c>
+      <c r="I69" s="5">
+        <v>250</v>
+      </c>
       <c r="J69" s="4" t="s">
         <v>63</v>
       </c>
@@ -5297,23 +5617,25 @@
       <c r="D70" s="6"/>
       <c r="E70" s="6"/>
       <c r="F70" s="5" t="s">
-        <v>118</v>
+        <v>926</v>
       </c>
       <c r="G70" s="5" t="s">
-        <v>646</v>
-      </c>
-      <c r="H70" s="5">
-        <v>80</v>
-      </c>
+        <v>927</v>
+      </c>
+      <c r="H70" s="5"/>
       <c r="I70" s="5"/>
       <c r="J70" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="K70" s="4"/>
-      <c r="L70" s="4"/>
+        <v>914</v>
+      </c>
+      <c r="K70" s="4" t="s">
+        <v>930</v>
+      </c>
+      <c r="L70" s="4" t="s">
+        <v>928</v>
+      </c>
       <c r="M70" s="4"/>
       <c r="N70" s="5" t="s">
-        <v>119</v>
+        <v>929</v>
       </c>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.25">
@@ -5323,17 +5645,17 @@
       <c r="D71" s="6"/>
       <c r="E71" s="6"/>
       <c r="F71" s="5" t="s">
-        <v>1027</v>
+        <v>674</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>1026</v>
+        <v>675</v>
       </c>
       <c r="H71" s="5">
-        <v>6000</v>
+        <v>50000</v>
       </c>
       <c r="I71" s="5"/>
       <c r="J71" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K71" s="4"/>
       <c r="L71" s="4"/>
@@ -5347,24 +5669,24 @@
       <c r="D72" s="6"/>
       <c r="E72" s="6"/>
       <c r="F72" s="5" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="G72" s="5" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="H72" s="5">
-        <v>150</v>
-      </c>
-      <c r="I72" s="5">
-        <v>75</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="I72" s="5"/>
       <c r="J72" s="4" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="K72" s="4"/>
       <c r="L72" s="4"/>
       <c r="M72" s="4"/>
-      <c r="N72" s="5"/>
+      <c r="N72" s="5" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="7"/>
@@ -5373,24 +5695,22 @@
       <c r="D73" s="6"/>
       <c r="E73" s="6"/>
       <c r="F73" s="5" t="s">
-        <v>980</v>
+        <v>1027</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>979</v>
+        <v>1026</v>
       </c>
       <c r="H73" s="5">
-        <v>1000</v>
+        <v>6000</v>
       </c>
       <c r="I73" s="5"/>
       <c r="J73" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K73" s="4"/>
       <c r="L73" s="4"/>
       <c r="M73" s="4"/>
-      <c r="N73" s="5" t="s">
-        <v>981</v>
-      </c>
+      <c r="N73" s="5"/>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="7"/>
@@ -5399,15 +5719,17 @@
       <c r="D74" s="6"/>
       <c r="E74" s="6"/>
       <c r="F74" s="5" t="s">
-        <v>978</v>
+        <v>128</v>
       </c>
       <c r="G74" s="5" t="s">
-        <v>977</v>
+        <v>647</v>
       </c>
       <c r="H74" s="5">
-        <v>600</v>
-      </c>
-      <c r="I74" s="5"/>
+        <v>150</v>
+      </c>
+      <c r="I74" s="5">
+        <v>75</v>
+      </c>
       <c r="J74" s="4" t="s">
         <v>63</v>
       </c>
@@ -5423,29 +5745,23 @@
       <c r="D75" s="6"/>
       <c r="E75" s="6"/>
       <c r="F75" s="5" t="s">
-        <v>84</v>
+        <v>980</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>18</v>
+        <v>979</v>
       </c>
       <c r="H75" s="5">
-        <v>75</v>
+        <v>1000</v>
       </c>
       <c r="I75" s="5"/>
       <c r="J75" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="K75" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="L75" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="M75" s="4" t="s">
-        <v>556</v>
-      </c>
+      <c r="K75" s="4"/>
+      <c r="L75" s="4"/>
+      <c r="M75" s="4"/>
       <c r="N75" s="5" t="s">
-        <v>116</v>
+        <v>981</v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.25">
@@ -5455,17 +5771,17 @@
       <c r="D76" s="6"/>
       <c r="E76" s="6"/>
       <c r="F76" s="5" t="s">
-        <v>112</v>
+        <v>978</v>
       </c>
       <c r="G76" s="5" t="s">
-        <v>30</v>
+        <v>977</v>
       </c>
       <c r="H76" s="5">
-        <v>1500</v>
+        <v>600</v>
       </c>
       <c r="I76" s="5"/>
       <c r="J76" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K76" s="4"/>
       <c r="L76" s="4"/>
@@ -5479,22 +5795,30 @@
       <c r="D77" s="6"/>
       <c r="E77" s="6"/>
       <c r="F77" s="5" t="s">
-        <v>203</v>
+        <v>84</v>
       </c>
       <c r="G77" s="5" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="H77" s="5">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="I77" s="5"/>
       <c r="J77" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K77" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="L77" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="K77" s="4"/>
-      <c r="L77" s="4"/>
-      <c r="M77" s="4"/>
-      <c r="N77" s="5"/>
+      <c r="M77" s="4" t="s">
+        <v>556</v>
+      </c>
+      <c r="N77" s="5" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="7"/>
@@ -5503,17 +5827,17 @@
       <c r="D78" s="6"/>
       <c r="E78" s="6"/>
       <c r="F78" s="5" t="s">
-        <v>919</v>
+        <v>112</v>
       </c>
       <c r="G78" s="5" t="s">
-        <v>918</v>
+        <v>30</v>
       </c>
       <c r="H78" s="5">
-        <v>400</v>
+        <v>1500</v>
       </c>
       <c r="I78" s="5"/>
       <c r="J78" s="4" t="s">
-        <v>694</v>
+        <v>62</v>
       </c>
       <c r="K78" s="4"/>
       <c r="L78" s="4"/>
@@ -5527,13 +5851,13 @@
       <c r="D79" s="6"/>
       <c r="E79" s="6"/>
       <c r="F79" s="5" t="s">
-        <v>691</v>
+        <v>203</v>
       </c>
       <c r="G79" s="5" t="s">
-        <v>986</v>
+        <v>55</v>
       </c>
       <c r="H79" s="5">
-        <v>400</v>
+        <v>30</v>
       </c>
       <c r="I79" s="5"/>
       <c r="J79" s="4" t="s">
@@ -5551,54 +5875,46 @@
       <c r="D80" s="6"/>
       <c r="E80" s="6"/>
       <c r="F80" s="5" t="s">
-        <v>129</v>
+        <v>919</v>
       </c>
       <c r="G80" s="5" t="s">
-        <v>722</v>
+        <v>918</v>
       </c>
       <c r="H80" s="5">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="I80" s="5"/>
       <c r="J80" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="K80" s="4" t="s">
         <v>694</v>
       </c>
-      <c r="L80" s="4" t="s">
-        <v>63</v>
-      </c>
+      <c r="K80" s="4"/>
+      <c r="L80" s="4"/>
       <c r="M80" s="4"/>
       <c r="N80" s="5"/>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" s="7"/>
-      <c r="B81" s="17"/>
+      <c r="B81" s="7"/>
       <c r="C81" s="7"/>
       <c r="D81" s="6"/>
       <c r="E81" s="6"/>
       <c r="F81" s="5" t="s">
-        <v>144</v>
+        <v>691</v>
       </c>
       <c r="G81" s="5" t="s">
-        <v>31</v>
+        <v>986</v>
       </c>
       <c r="H81" s="5">
-        <v>2000</v>
-      </c>
-      <c r="I81" s="5">
-        <v>200</v>
-      </c>
+        <v>400</v>
+      </c>
+      <c r="I81" s="5"/>
       <c r="J81" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K81" s="4"/>
       <c r="L81" s="4"/>
       <c r="M81" s="4"/>
-      <c r="N81" s="5" t="s">
-        <v>644</v>
-      </c>
+      <c r="N81" s="5"/>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" s="7"/>
@@ -5607,63 +5923,75 @@
       <c r="D82" s="6"/>
       <c r="E82" s="6"/>
       <c r="F82" s="5" t="s">
-        <v>92</v>
+        <v>129</v>
       </c>
       <c r="G82" s="5" t="s">
-        <v>32</v>
+        <v>722</v>
       </c>
       <c r="H82" s="5">
         <v>500</v>
       </c>
-      <c r="I82" s="5">
-        <v>1000</v>
-      </c>
+      <c r="I82" s="5"/>
       <c r="J82" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="K82" s="4"/>
-      <c r="L82" s="4"/>
+        <v>66</v>
+      </c>
+      <c r="K82" s="4" t="s">
+        <v>694</v>
+      </c>
+      <c r="L82" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="M82" s="4"/>
       <c r="N82" s="5"/>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" s="7"/>
-      <c r="B83" s="7"/>
+      <c r="B83" s="17"/>
       <c r="C83" s="7"/>
       <c r="D83" s="6"/>
-      <c r="E83" s="5"/>
+      <c r="E83" s="6"/>
       <c r="F83" s="5" t="s">
-        <v>775</v>
+        <v>144</v>
       </c>
       <c r="G83" s="5" t="s">
-        <v>790</v>
-      </c>
-      <c r="H83" s="5"/>
-      <c r="I83" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="H83" s="5">
+        <v>2000</v>
+      </c>
+      <c r="I83" s="5">
+        <v>200</v>
+      </c>
       <c r="J83" s="4" t="s">
-        <v>694</v>
+        <v>62</v>
       </c>
       <c r="K83" s="4"/>
       <c r="L83" s="4"/>
       <c r="M83" s="4"/>
-      <c r="N83" s="5"/>
+      <c r="N83" s="5" t="s">
+        <v>644</v>
+      </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" s="7"/>
       <c r="B84" s="7"/>
       <c r="C84" s="7"/>
       <c r="D84" s="6"/>
-      <c r="E84" s="5"/>
+      <c r="E84" s="6"/>
       <c r="F84" s="5" t="s">
-        <v>774</v>
+        <v>92</v>
       </c>
       <c r="G84" s="5" t="s">
-        <v>789</v>
-      </c>
-      <c r="H84" s="5"/>
-      <c r="I84" s="5"/>
+        <v>32</v>
+      </c>
+      <c r="H84" s="5">
+        <v>500</v>
+      </c>
+      <c r="I84" s="5">
+        <v>1000</v>
+      </c>
       <c r="J84" s="4" t="s">
-        <v>694</v>
+        <v>62</v>
       </c>
       <c r="K84" s="4"/>
       <c r="L84" s="4"/>
@@ -5677,10 +6005,10 @@
       <c r="D85" s="6"/>
       <c r="E85" s="5"/>
       <c r="F85" s="5" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="G85" s="5" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="H85" s="5"/>
       <c r="I85" s="5"/>
@@ -5699,17 +6027,15 @@
       <c r="D86" s="6"/>
       <c r="E86" s="5"/>
       <c r="F86" s="5" t="s">
-        <v>474</v>
+        <v>774</v>
       </c>
       <c r="G86" s="5" t="s">
-        <v>1028</v>
-      </c>
-      <c r="H86" s="5">
-        <v>2000</v>
-      </c>
+        <v>789</v>
+      </c>
+      <c r="H86" s="5"/>
       <c r="I86" s="5"/>
       <c r="J86" s="4" t="s">
-        <v>474</v>
+        <v>694</v>
       </c>
       <c r="K86" s="4"/>
       <c r="L86" s="4"/>
@@ -5723,21 +6049,17 @@
       <c r="D87" s="6"/>
       <c r="E87" s="5"/>
       <c r="F87" s="5" t="s">
-        <v>728</v>
+        <v>776</v>
       </c>
       <c r="G87" s="5" t="s">
-        <v>725</v>
-      </c>
-      <c r="H87" s="5">
-        <v>280</v>
-      </c>
+        <v>791</v>
+      </c>
+      <c r="H87" s="5"/>
       <c r="I87" s="5"/>
       <c r="J87" s="4" t="s">
-        <v>417</v>
-      </c>
-      <c r="K87" s="4" t="s">
         <v>694</v>
       </c>
+      <c r="K87" s="4"/>
       <c r="L87" s="4"/>
       <c r="M87" s="4"/>
       <c r="N87" s="5"/>
@@ -5749,146 +6071,142 @@
       <c r="D88" s="6"/>
       <c r="E88" s="5"/>
       <c r="F88" s="5" t="s">
-        <v>739</v>
+        <v>474</v>
       </c>
       <c r="G88" s="5" t="s">
-        <v>740</v>
+        <v>1028</v>
       </c>
       <c r="H88" s="5">
-        <v>600</v>
+        <v>2000</v>
       </c>
       <c r="I88" s="5"/>
       <c r="J88" s="4" t="s">
-        <v>556</v>
-      </c>
-      <c r="K88" s="4" t="s">
-        <v>694</v>
-      </c>
+        <v>474</v>
+      </c>
+      <c r="K88" s="4"/>
       <c r="L88" s="4"/>
       <c r="M88" s="4"/>
       <c r="N88" s="5"/>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" s="7"/>
-      <c r="B89" s="18"/>
+      <c r="B89" s="7"/>
       <c r="C89" s="7"/>
       <c r="D89" s="6"/>
-      <c r="E89" s="6"/>
+      <c r="E89" s="5"/>
       <c r="F89" s="5" t="s">
-        <v>671</v>
+        <v>728</v>
       </c>
       <c r="G89" s="5" t="s">
-        <v>670</v>
+        <v>725</v>
       </c>
       <c r="H89" s="5">
-        <v>50000</v>
+        <v>280</v>
       </c>
       <c r="I89" s="5"/>
       <c r="J89" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="K89" s="4"/>
+        <v>417</v>
+      </c>
+      <c r="K89" s="4" t="s">
+        <v>694</v>
+      </c>
       <c r="L89" s="4"/>
       <c r="M89" s="4"/>
-      <c r="N89" s="5" t="s">
-        <v>1012</v>
-      </c>
+      <c r="N89" s="5"/>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" s="7"/>
-      <c r="B90" s="6"/>
+      <c r="B90" s="7"/>
       <c r="C90" s="7"/>
       <c r="D90" s="6"/>
-      <c r="E90" s="6"/>
+      <c r="E90" s="5"/>
       <c r="F90" s="5" t="s">
-        <v>898</v>
+        <v>739</v>
       </c>
       <c r="G90" s="5" t="s">
-        <v>896</v>
+        <v>740</v>
       </c>
       <c r="H90" s="5">
-        <v>80</v>
+        <v>600</v>
       </c>
       <c r="I90" s="5"/>
       <c r="J90" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="K90" s="4"/>
+        <v>556</v>
+      </c>
+      <c r="K90" s="4" t="s">
+        <v>694</v>
+      </c>
       <c r="L90" s="4"/>
       <c r="M90" s="4"/>
-      <c r="N90" s="5" t="s">
-        <v>897</v>
-      </c>
+      <c r="N90" s="5"/>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" s="7"/>
-      <c r="B91" s="7"/>
+      <c r="B91" s="18"/>
       <c r="C91" s="7"/>
       <c r="D91" s="6"/>
       <c r="E91" s="6"/>
       <c r="F91" s="5" t="s">
-        <v>1024</v>
+        <v>671</v>
       </c>
       <c r="G91" s="5" t="s">
-        <v>1023</v>
+        <v>670</v>
       </c>
       <c r="H91" s="5">
-        <v>200</v>
+        <v>50000</v>
       </c>
       <c r="I91" s="5"/>
       <c r="J91" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K91" s="4"/>
       <c r="L91" s="4"/>
       <c r="M91" s="4"/>
-      <c r="N91" s="5"/>
+      <c r="N91" s="5" t="s">
+        <v>1012</v>
+      </c>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" s="7"/>
-      <c r="B92" s="7"/>
+      <c r="B92" s="6"/>
       <c r="C92" s="7"/>
       <c r="D92" s="6"/>
       <c r="E92" s="6"/>
       <c r="F92" s="5" t="s">
-        <v>85</v>
+        <v>898</v>
       </c>
       <c r="G92" s="5" t="s">
-        <v>107</v>
+        <v>896</v>
       </c>
       <c r="H92" s="5">
-        <v>200</v>
-      </c>
-      <c r="I92" s="5">
-        <v>250</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="I92" s="5"/>
       <c r="J92" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="K92" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="L92" s="4" t="s">
-        <v>63</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="K92" s="4"/>
+      <c r="L92" s="4"/>
       <c r="M92" s="4"/>
       <c r="N92" s="5" t="s">
-        <v>642</v>
+        <v>897</v>
       </c>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A93" s="6"/>
-      <c r="B93" s="6"/>
-      <c r="C93" s="6"/>
+      <c r="A93" s="7"/>
+      <c r="B93" s="7"/>
+      <c r="C93" s="7"/>
       <c r="D93" s="6"/>
-      <c r="E93" s="5"/>
+      <c r="E93" s="6"/>
       <c r="F93" s="5" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="G93" s="5" t="s">
-        <v>976</v>
-      </c>
-      <c r="H93" s="5"/>
+        <v>1023</v>
+      </c>
+      <c r="H93" s="5">
+        <v>200</v>
+      </c>
       <c r="I93" s="5"/>
       <c r="J93" s="4" t="s">
         <v>65</v>
@@ -5896,92 +6214,88 @@
       <c r="K93" s="4"/>
       <c r="L93" s="4"/>
       <c r="M93" s="4"/>
-      <c r="N93" s="5" t="s">
-        <v>960</v>
-      </c>
+      <c r="N93" s="5"/>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A94" s="6"/>
-      <c r="B94" s="6"/>
-      <c r="C94" s="6"/>
+      <c r="A94" s="7"/>
+      <c r="B94" s="7"/>
+      <c r="C94" s="7"/>
       <c r="D94" s="6"/>
-      <c r="E94" s="5"/>
+      <c r="E94" s="6"/>
       <c r="F94" s="5" t="s">
-        <v>961</v>
+        <v>85</v>
       </c>
       <c r="G94" s="5" t="s">
-        <v>962</v>
+        <v>107</v>
       </c>
       <c r="H94" s="5">
         <v>200</v>
       </c>
-      <c r="I94" s="5"/>
+      <c r="I94" s="5">
+        <v>250</v>
+      </c>
       <c r="J94" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="K94" s="4"/>
-      <c r="L94" s="4"/>
+        <v>61</v>
+      </c>
+      <c r="K94" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="L94" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="M94" s="4"/>
       <c r="N94" s="5" t="s">
-        <v>960</v>
+        <v>642</v>
       </c>
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A95" s="7"/>
-      <c r="B95" s="7"/>
-      <c r="C95" s="7"/>
+      <c r="A95" s="6"/>
+      <c r="B95" s="6"/>
+      <c r="C95" s="6"/>
       <c r="D95" s="6"/>
-      <c r="E95" s="6"/>
+      <c r="E95" s="5"/>
       <c r="F95" s="5" t="s">
-        <v>641</v>
+        <v>1025</v>
       </c>
       <c r="G95" s="5" t="s">
-        <v>640</v>
-      </c>
-      <c r="H95" s="5">
-        <v>200</v>
-      </c>
+        <v>976</v>
+      </c>
+      <c r="H95" s="5"/>
       <c r="I95" s="5"/>
       <c r="J95" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="K95" s="4" t="s">
         <v>65</v>
       </c>
+      <c r="K95" s="4"/>
       <c r="L95" s="4"/>
       <c r="M95" s="4"/>
-      <c r="N95" s="5"/>
+      <c r="N95" s="5" t="s">
+        <v>960</v>
+      </c>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A96" s="7"/>
-      <c r="B96" s="7"/>
-      <c r="C96" s="7"/>
+      <c r="A96" s="6"/>
+      <c r="B96" s="6"/>
+      <c r="C96" s="6"/>
       <c r="D96" s="6"/>
-      <c r="E96" s="6"/>
+      <c r="E96" s="5"/>
       <c r="F96" s="5" t="s">
-        <v>639</v>
+        <v>961</v>
       </c>
       <c r="G96" s="5" t="s">
-        <v>138</v>
+        <v>962</v>
       </c>
       <c r="H96" s="5">
         <v>200</v>
       </c>
-      <c r="I96" s="5">
-        <v>250</v>
-      </c>
+      <c r="I96" s="5"/>
       <c r="J96" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="K96" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="L96" s="4" t="s">
         <v>65</v>
       </c>
+      <c r="K96" s="4"/>
+      <c r="L96" s="4"/>
       <c r="M96" s="4"/>
       <c r="N96" s="5" t="s">
-        <v>643</v>
+        <v>960</v>
       </c>
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.25">
@@ -5991,19 +6305,21 @@
       <c r="D97" s="6"/>
       <c r="E97" s="6"/>
       <c r="F97" s="5" t="s">
-        <v>110</v>
+        <v>641</v>
       </c>
       <c r="G97" s="5" t="s">
-        <v>19</v>
+        <v>640</v>
       </c>
       <c r="H97" s="5">
-        <v>50000</v>
+        <v>200</v>
       </c>
       <c r="I97" s="5"/>
       <c r="J97" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="K97" s="4"/>
+        <v>62</v>
+      </c>
+      <c r="K97" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="L97" s="4"/>
       <c r="M97" s="4"/>
       <c r="N97" s="5"/>
@@ -6015,22 +6331,30 @@
       <c r="D98" s="6"/>
       <c r="E98" s="6"/>
       <c r="F98" s="5" t="s">
-        <v>997</v>
+        <v>639</v>
       </c>
       <c r="G98" s="5" t="s">
-        <v>998</v>
+        <v>138</v>
       </c>
       <c r="H98" s="5">
-        <v>135</v>
-      </c>
-      <c r="I98" s="5"/>
+        <v>200</v>
+      </c>
+      <c r="I98" s="5">
+        <v>250</v>
+      </c>
       <c r="J98" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="K98" s="4"/>
-      <c r="L98" s="4"/>
+        <v>66</v>
+      </c>
+      <c r="K98" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="L98" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="M98" s="4"/>
-      <c r="N98" s="5"/>
+      <c r="N98" s="5" t="s">
+        <v>643</v>
+      </c>
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99" s="7"/>
@@ -6039,17 +6363,17 @@
       <c r="D99" s="6"/>
       <c r="E99" s="6"/>
       <c r="F99" s="5" t="s">
-        <v>852</v>
+        <v>110</v>
       </c>
       <c r="G99" s="5" t="s">
-        <v>853</v>
+        <v>19</v>
       </c>
       <c r="H99" s="5">
-        <v>150</v>
+        <v>50000</v>
       </c>
       <c r="I99" s="5"/>
       <c r="J99" s="4" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="K99" s="4"/>
       <c r="L99" s="4"/>
@@ -6063,17 +6387,17 @@
       <c r="D100" s="6"/>
       <c r="E100" s="6"/>
       <c r="F100" s="5" t="s">
-        <v>140</v>
+        <v>997</v>
       </c>
       <c r="G100" s="5" t="s">
-        <v>141</v>
+        <v>998</v>
       </c>
       <c r="H100" s="5">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="I100" s="5"/>
       <c r="J100" s="4" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="K100" s="4"/>
       <c r="L100" s="4"/>
@@ -6087,22 +6411,22 @@
       <c r="D101" s="6"/>
       <c r="E101" s="6"/>
       <c r="F101" s="5" t="s">
-        <v>1018</v>
+        <v>852</v>
       </c>
       <c r="G101" s="5" t="s">
-        <v>963</v>
-      </c>
-      <c r="H101" s="5"/>
+        <v>853</v>
+      </c>
+      <c r="H101" s="5">
+        <v>150</v>
+      </c>
       <c r="I101" s="5"/>
       <c r="J101" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="K101" s="4"/>
       <c r="L101" s="4"/>
       <c r="M101" s="4"/>
-      <c r="N101" s="5" t="s">
-        <v>960</v>
-      </c>
+      <c r="N101" s="5"/>
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A102" s="7"/>
@@ -6111,17 +6435,17 @@
       <c r="D102" s="6"/>
       <c r="E102" s="6"/>
       <c r="F102" s="5" t="s">
-        <v>806</v>
+        <v>140</v>
       </c>
       <c r="G102" s="5" t="s">
-        <v>807</v>
+        <v>141</v>
       </c>
       <c r="H102" s="5">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="I102" s="5"/>
       <c r="J102" s="4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="K102" s="4"/>
       <c r="L102" s="4"/>
@@ -6135,27 +6459,21 @@
       <c r="D103" s="6"/>
       <c r="E103" s="6"/>
       <c r="F103" s="5" t="s">
-        <v>130</v>
+        <v>1018</v>
       </c>
       <c r="G103" s="5" t="s">
-        <v>590</v>
-      </c>
-      <c r="H103" s="5">
-        <v>100</v>
-      </c>
+        <v>963</v>
+      </c>
+      <c r="H103" s="5"/>
       <c r="I103" s="5"/>
       <c r="J103" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="K103" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="L103" s="4" t="s">
-        <v>63</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="K103" s="4"/>
+      <c r="L103" s="4"/>
       <c r="M103" s="4"/>
       <c r="N103" s="5" t="s">
-        <v>591</v>
+        <v>960</v>
       </c>
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.25">
@@ -6163,19 +6481,19 @@
       <c r="B104" s="7"/>
       <c r="C104" s="7"/>
       <c r="D104" s="6"/>
-      <c r="E104" s="5"/>
+      <c r="E104" s="6"/>
       <c r="F104" s="5" t="s">
-        <v>920</v>
+        <v>806</v>
       </c>
       <c r="G104" s="5" t="s">
-        <v>921</v>
+        <v>807</v>
       </c>
       <c r="H104" s="5">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="I104" s="5"/>
       <c r="J104" s="4" t="s">
-        <v>694</v>
+        <v>63</v>
       </c>
       <c r="K104" s="4"/>
       <c r="L104" s="4"/>
@@ -6187,24 +6505,30 @@
       <c r="B105" s="7"/>
       <c r="C105" s="7"/>
       <c r="D105" s="6"/>
-      <c r="E105" s="5"/>
+      <c r="E105" s="6"/>
       <c r="F105" s="5" t="s">
-        <v>1000</v>
+        <v>130</v>
       </c>
       <c r="G105" s="5" t="s">
-        <v>999</v>
+        <v>590</v>
       </c>
       <c r="H105" s="5">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="I105" s="5"/>
       <c r="J105" s="4" t="s">
-        <v>992</v>
-      </c>
-      <c r="K105" s="4"/>
-      <c r="L105" s="4"/>
+        <v>68</v>
+      </c>
+      <c r="K105" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="L105" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="M105" s="4"/>
-      <c r="N105" s="5"/>
+      <c r="N105" s="5" t="s">
+        <v>591</v>
+      </c>
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A106" s="7"/>
@@ -6213,26 +6537,22 @@
       <c r="D106" s="6"/>
       <c r="E106" s="5"/>
       <c r="F106" s="5" t="s">
-        <v>91</v>
+        <v>920</v>
       </c>
       <c r="G106" s="5" t="s">
-        <v>729</v>
+        <v>921</v>
       </c>
       <c r="H106" s="5">
-        <v>750</v>
+        <v>200</v>
       </c>
       <c r="I106" s="5"/>
       <c r="J106" s="4" t="s">
-        <v>556</v>
-      </c>
-      <c r="K106" s="4" t="s">
         <v>694</v>
       </c>
+      <c r="K106" s="4"/>
       <c r="L106" s="4"/>
       <c r="M106" s="4"/>
-      <c r="N106" s="5" t="s">
-        <v>737</v>
-      </c>
+      <c r="N106" s="5"/>
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A107" s="7"/>
@@ -6241,21 +6561,19 @@
       <c r="D107" s="6"/>
       <c r="E107" s="5"/>
       <c r="F107" s="5" t="s">
-        <v>738</v>
+        <v>1000</v>
       </c>
       <c r="G107" s="5" t="s">
-        <v>730</v>
+        <v>999</v>
       </c>
       <c r="H107" s="5">
-        <v>3000</v>
+        <v>200</v>
       </c>
       <c r="I107" s="5"/>
       <c r="J107" s="4" t="s">
-        <v>556</v>
-      </c>
-      <c r="K107" s="4" t="s">
-        <v>694</v>
-      </c>
+        <v>992</v>
+      </c>
+      <c r="K107" s="4"/>
       <c r="L107" s="4"/>
       <c r="M107" s="4"/>
       <c r="N107" s="5"/>
@@ -6265,54 +6583,54 @@
       <c r="B108" s="7"/>
       <c r="C108" s="7"/>
       <c r="D108" s="6"/>
-      <c r="E108" s="6"/>
+      <c r="E108" s="5"/>
       <c r="F108" s="5" t="s">
-        <v>131</v>
+        <v>91</v>
       </c>
       <c r="G108" s="5" t="s">
-        <v>56</v>
+        <v>729</v>
       </c>
       <c r="H108" s="5">
-        <v>80</v>
-      </c>
-      <c r="I108" s="5">
-        <v>120</v>
-      </c>
+        <v>750</v>
+      </c>
+      <c r="I108" s="5"/>
       <c r="J108" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="K108" s="4"/>
+        <v>556</v>
+      </c>
+      <c r="K108" s="4" t="s">
+        <v>694</v>
+      </c>
       <c r="L108" s="4"/>
       <c r="M108" s="4"/>
-      <c r="N108" s="5"/>
+      <c r="N108" s="5" t="s">
+        <v>737</v>
+      </c>
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A109" s="7"/>
       <c r="B109" s="7"/>
       <c r="C109" s="7"/>
-      <c r="D109" s="7"/>
-      <c r="E109" s="6"/>
+      <c r="D109" s="6"/>
+      <c r="E109" s="5"/>
       <c r="F109" s="5" t="s">
-        <v>139</v>
+        <v>738</v>
       </c>
       <c r="G109" s="5" t="s">
-        <v>27</v>
+        <v>730</v>
       </c>
       <c r="H109" s="5">
-        <v>300</v>
+        <v>3000</v>
       </c>
       <c r="I109" s="5"/>
       <c r="J109" s="4" t="s">
-        <v>64</v>
+        <v>556</v>
       </c>
       <c r="K109" s="4" t="s">
-        <v>67</v>
+        <v>694</v>
       </c>
       <c r="L109" s="4"/>
       <c r="M109" s="4"/>
-      <c r="N109" s="5" t="s">
-        <v>592</v>
-      </c>
+      <c r="N109" s="5"/>
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A110" s="7"/>
@@ -6321,54 +6639,52 @@
       <c r="D110" s="6"/>
       <c r="E110" s="6"/>
       <c r="F110" s="5" t="s">
-        <v>660</v>
+        <v>131</v>
       </c>
       <c r="G110" s="5" t="s">
-        <v>661</v>
+        <v>56</v>
       </c>
       <c r="H110" s="5">
-        <v>500</v>
+        <v>80</v>
       </c>
       <c r="I110" s="5">
-        <v>400</v>
+        <v>120</v>
       </c>
       <c r="J110" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="K110" s="4" t="s">
         <v>63</v>
       </c>
+      <c r="K110" s="4"/>
       <c r="L110" s="4"/>
       <c r="M110" s="4"/>
-      <c r="N110" s="5" t="s">
-        <v>662</v>
-      </c>
+      <c r="N110" s="5"/>
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A111" s="7"/>
       <c r="B111" s="7"/>
       <c r="C111" s="7"/>
-      <c r="D111" s="6"/>
+      <c r="D111" s="7"/>
       <c r="E111" s="6"/>
       <c r="F111" s="5" t="s">
-        <v>109</v>
+        <v>139</v>
       </c>
       <c r="G111" s="5" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="H111" s="5">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="I111" s="5"/>
       <c r="J111" s="4" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="K111" s="4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="L111" s="4"/>
       <c r="M111" s="4"/>
-      <c r="N111" s="5"/>
+      <c r="N111" s="5" t="s">
+        <v>592</v>
+      </c>
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A112" s="7"/>
@@ -6377,25 +6693,27 @@
       <c r="D112" s="6"/>
       <c r="E112" s="6"/>
       <c r="F112" s="5" t="s">
-        <v>109</v>
+        <v>660</v>
       </c>
       <c r="G112" s="5" t="s">
-        <v>995</v>
+        <v>661</v>
       </c>
       <c r="H112" s="5">
-        <v>2500</v>
+        <v>500</v>
       </c>
       <c r="I112" s="5">
-        <v>4300</v>
+        <v>400</v>
       </c>
       <c r="J112" s="4" t="s">
-        <v>992</v>
-      </c>
-      <c r="K112" s="4"/>
+        <v>68</v>
+      </c>
+      <c r="K112" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="L112" s="4"/>
       <c r="M112" s="4"/>
       <c r="N112" s="5" t="s">
-        <v>996</v>
+        <v>662</v>
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.25">
@@ -6405,19 +6723,21 @@
       <c r="D113" s="6"/>
       <c r="E113" s="6"/>
       <c r="F113" s="5" t="s">
-        <v>86</v>
+        <v>109</v>
       </c>
       <c r="G113" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H113" s="5">
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="I113" s="5"/>
       <c r="J113" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="K113" s="4"/>
+      <c r="K113" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="L113" s="4"/>
       <c r="M113" s="4"/>
       <c r="N113" s="5"/>
@@ -6429,22 +6749,26 @@
       <c r="D114" s="6"/>
       <c r="E114" s="6"/>
       <c r="F114" s="5" t="s">
-        <v>1019</v>
+        <v>109</v>
       </c>
       <c r="G114" s="5" t="s">
-        <v>1017</v>
+        <v>995</v>
       </c>
       <c r="H114" s="5">
-        <v>150</v>
-      </c>
-      <c r="I114" s="5"/>
+        <v>2500</v>
+      </c>
+      <c r="I114" s="5">
+        <v>4300</v>
+      </c>
       <c r="J114" s="4" t="s">
-        <v>914</v>
+        <v>992</v>
       </c>
       <c r="K114" s="4"/>
       <c r="L114" s="4"/>
       <c r="M114" s="4"/>
-      <c r="N114" s="5"/>
+      <c r="N114" s="5" t="s">
+        <v>996</v>
+      </c>
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A115" s="7"/>
@@ -6453,17 +6777,17 @@
       <c r="D115" s="6"/>
       <c r="E115" s="6"/>
       <c r="F115" s="5" t="s">
-        <v>204</v>
+        <v>86</v>
       </c>
       <c r="G115" s="5" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="H115" s="5">
-        <v>120</v>
+        <v>600</v>
       </c>
       <c r="I115" s="5"/>
       <c r="J115" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K115" s="4"/>
       <c r="L115" s="4"/>
@@ -6477,14 +6801,18 @@
       <c r="D116" s="6"/>
       <c r="E116" s="6"/>
       <c r="F116" s="5" t="s">
-        <v>751</v>
+        <v>1019</v>
       </c>
       <c r="G116" s="5" t="s">
-        <v>750</v>
-      </c>
-      <c r="H116" s="5"/>
+        <v>1017</v>
+      </c>
+      <c r="H116" s="5">
+        <v>150</v>
+      </c>
       <c r="I116" s="5"/>
-      <c r="J116" s="4"/>
+      <c r="J116" s="4" t="s">
+        <v>914</v>
+      </c>
       <c r="K116" s="4"/>
       <c r="L116" s="4"/>
       <c r="M116" s="4"/>
@@ -6497,23 +6825,19 @@
       <c r="D117" s="6"/>
       <c r="E117" s="6"/>
       <c r="F117" s="5" t="s">
-        <v>94</v>
+        <v>204</v>
       </c>
       <c r="G117" s="5" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="H117" s="5">
-        <v>30</v>
-      </c>
-      <c r="I117" s="5">
-        <v>75</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="I117" s="5"/>
       <c r="J117" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="K117" s="4" t="s">
         <v>63</v>
       </c>
+      <c r="K117" s="4"/>
       <c r="L117" s="4"/>
       <c r="M117" s="4"/>
       <c r="N117" s="5"/>
@@ -6525,50 +6849,44 @@
       <c r="D118" s="6"/>
       <c r="E118" s="6"/>
       <c r="F118" s="5" t="s">
-        <v>90</v>
+        <v>751</v>
       </c>
       <c r="G118" s="5" t="s">
-        <v>372</v>
-      </c>
-      <c r="H118" s="5">
-        <v>200</v>
-      </c>
+        <v>750</v>
+      </c>
+      <c r="H118" s="5"/>
       <c r="I118" s="5"/>
-      <c r="J118" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="K118" s="4" t="s">
-        <v>65</v>
-      </c>
+      <c r="J118" s="4"/>
+      <c r="K118" s="4"/>
       <c r="L118" s="4"/>
       <c r="M118" s="4"/>
-      <c r="N118" s="5" t="s">
-        <v>589</v>
-      </c>
+      <c r="N118" s="5"/>
     </row>
     <row r="119" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A119" s="7"/>
       <c r="B119" s="7"/>
       <c r="C119" s="7"/>
       <c r="D119" s="6"/>
-      <c r="E119" s="5"/>
+      <c r="E119" s="6"/>
       <c r="F119" s="5" t="s">
-        <v>724</v>
+        <v>1103</v>
       </c>
       <c r="G119" s="5" t="s">
-        <v>723</v>
+        <v>1101</v>
       </c>
       <c r="H119" s="5">
-        <v>350</v>
+        <v>2400</v>
       </c>
       <c r="I119" s="5"/>
       <c r="J119" s="4" t="s">
-        <v>66</v>
+        <v>1060</v>
       </c>
       <c r="K119" s="4"/>
       <c r="L119" s="4"/>
       <c r="M119" s="4"/>
-      <c r="N119" s="5"/>
+      <c r="N119" s="5" t="s">
+        <v>1102</v>
+      </c>
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A120" s="7"/>
@@ -6577,71 +6895,75 @@
       <c r="D120" s="6"/>
       <c r="E120" s="6"/>
       <c r="F120" s="5" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="G120" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H120" s="5">
-        <v>1000</v>
-      </c>
-      <c r="I120" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="I120" s="5">
+        <v>75</v>
+      </c>
       <c r="J120" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="K120" s="4"/>
+        <v>66</v>
+      </c>
+      <c r="K120" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="L120" s="4"/>
       <c r="M120" s="4"/>
       <c r="N120" s="5"/>
     </row>
     <row r="121" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A121" s="7"/>
-      <c r="B121" s="6"/>
+      <c r="B121" s="7"/>
       <c r="C121" s="7"/>
       <c r="D121" s="6"/>
       <c r="E121" s="6"/>
       <c r="F121" s="5" t="s">
-        <v>983</v>
+        <v>90</v>
       </c>
       <c r="G121" s="5" t="s">
-        <v>982</v>
+        <v>372</v>
       </c>
       <c r="H121" s="5">
         <v>200</v>
       </c>
       <c r="I121" s="5"/>
       <c r="J121" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="K121" s="4"/>
+        <v>64</v>
+      </c>
+      <c r="K121" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="L121" s="4"/>
       <c r="M121" s="4"/>
-      <c r="N121" s="5"/>
+      <c r="N121" s="5" t="s">
+        <v>589</v>
+      </c>
     </row>
     <row r="122" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A122" s="7"/>
       <c r="B122" s="7"/>
       <c r="C122" s="7"/>
       <c r="D122" s="6"/>
-      <c r="E122" s="6"/>
+      <c r="E122" s="5"/>
       <c r="F122" s="5" t="s">
-        <v>666</v>
+        <v>724</v>
       </c>
       <c r="G122" s="5" t="s">
-        <v>665</v>
+        <v>723</v>
       </c>
       <c r="H122" s="5">
-        <v>30</v>
-      </c>
-      <c r="I122" s="5">
-        <v>60</v>
-      </c>
+        <v>350</v>
+      </c>
+      <c r="I122" s="5"/>
       <c r="J122" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="K122" s="4" t="s">
-        <v>63</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="K122" s="4"/>
       <c r="L122" s="4"/>
       <c r="M122" s="4"/>
       <c r="N122" s="5"/>
@@ -6653,13 +6975,13 @@
       <c r="D123" s="6"/>
       <c r="E123" s="6"/>
       <c r="F123" s="5" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="G123" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H123" s="5">
-        <v>150</v>
+        <v>1000</v>
       </c>
       <c r="I123" s="5"/>
       <c r="J123" s="4" t="s">
@@ -6672,26 +6994,24 @@
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A124" s="7"/>
-      <c r="B124" s="7"/>
+      <c r="B124" s="6"/>
       <c r="C124" s="7"/>
       <c r="D124" s="6"/>
       <c r="E124" s="6"/>
       <c r="F124" s="5" t="s">
-        <v>108</v>
+        <v>983</v>
       </c>
       <c r="G124" s="5" t="s">
-        <v>22</v>
+        <v>982</v>
       </c>
       <c r="H124" s="5">
-        <v>80</v>
+        <v>200</v>
       </c>
       <c r="I124" s="5"/>
       <c r="J124" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="K124" s="4" t="s">
-        <v>62</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="K124" s="4"/>
       <c r="L124" s="4"/>
       <c r="M124" s="4"/>
       <c r="N124" s="5"/>
@@ -6703,49 +7023,47 @@
       <c r="D125" s="6"/>
       <c r="E125" s="6"/>
       <c r="F125" s="5" t="s">
-        <v>636</v>
+        <v>666</v>
       </c>
       <c r="G125" s="5" t="s">
-        <v>638</v>
+        <v>665</v>
       </c>
       <c r="H125" s="5">
-        <v>100</v>
-      </c>
-      <c r="I125" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="I125" s="5">
+        <v>60</v>
+      </c>
       <c r="J125" s="4" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="K125" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L125" s="4"/>
       <c r="M125" s="4"/>
-      <c r="N125" s="5" t="s">
-        <v>115</v>
-      </c>
+      <c r="N125" s="5"/>
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A126" s="7"/>
       <c r="B126" s="7"/>
       <c r="C126" s="7"/>
       <c r="D126" s="6"/>
-      <c r="E126" s="5"/>
+      <c r="E126" s="6"/>
       <c r="F126" s="5" t="s">
-        <v>727</v>
+        <v>114</v>
       </c>
       <c r="G126" s="5" t="s">
-        <v>726</v>
+        <v>34</v>
       </c>
       <c r="H126" s="5">
-        <v>1600</v>
+        <v>150</v>
       </c>
       <c r="I126" s="5"/>
       <c r="J126" s="4" t="s">
-        <v>417</v>
-      </c>
-      <c r="K126" s="4" t="s">
-        <v>694</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="K126" s="4"/>
       <c r="L126" s="4"/>
       <c r="M126" s="4"/>
       <c r="N126" s="5"/>
@@ -6757,19 +7075,21 @@
       <c r="D127" s="6"/>
       <c r="E127" s="6"/>
       <c r="F127" s="5" t="s">
-        <v>136</v>
+        <v>108</v>
       </c>
       <c r="G127" s="5" t="s">
-        <v>137</v>
+        <v>22</v>
       </c>
       <c r="H127" s="5">
-        <v>3000</v>
+        <v>80</v>
       </c>
       <c r="I127" s="5"/>
       <c r="J127" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="K127" s="4"/>
+        <v>61</v>
+      </c>
+      <c r="K127" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="L127" s="4"/>
       <c r="M127" s="4"/>
       <c r="N127" s="5"/>
@@ -6781,41 +7101,45 @@
       <c r="D128" s="6"/>
       <c r="E128" s="6"/>
       <c r="F128" s="5" t="s">
-        <v>753</v>
+        <v>636</v>
       </c>
       <c r="G128" s="5" t="s">
-        <v>754</v>
+        <v>638</v>
       </c>
       <c r="H128" s="5">
-        <v>1800</v>
+        <v>100</v>
       </c>
       <c r="I128" s="5"/>
       <c r="J128" s="4" t="s">
-        <v>755</v>
-      </c>
-      <c r="K128" s="4"/>
+        <v>61</v>
+      </c>
+      <c r="K128" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="L128" s="4"/>
       <c r="M128" s="4"/>
-      <c r="N128" s="5"/>
+      <c r="N128" s="5" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="129" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A129" s="7"/>
       <c r="B129" s="7"/>
       <c r="C129" s="7"/>
       <c r="D129" s="6"/>
-      <c r="E129" s="6"/>
+      <c r="E129" s="5"/>
       <c r="F129" s="5" t="s">
-        <v>915</v>
+        <v>727</v>
       </c>
       <c r="G129" s="5" t="s">
-        <v>917</v>
+        <v>726</v>
       </c>
       <c r="H129" s="5">
-        <v>400</v>
+        <v>1600</v>
       </c>
       <c r="I129" s="5"/>
       <c r="J129" s="4" t="s">
-        <v>916</v>
+        <v>417</v>
       </c>
       <c r="K129" s="4" t="s">
         <v>694</v>
@@ -6831,21 +7155,19 @@
       <c r="D130" s="6"/>
       <c r="E130" s="6"/>
       <c r="F130" s="5" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="G130" s="5" t="s">
-        <v>42</v>
+        <v>137</v>
       </c>
       <c r="H130" s="5">
-        <v>30</v>
+        <v>3000</v>
       </c>
       <c r="I130" s="5"/>
       <c r="J130" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="K130" s="4" t="s">
-        <v>63</v>
-      </c>
+      <c r="K130" s="4"/>
       <c r="L130" s="4"/>
       <c r="M130" s="4"/>
       <c r="N130" s="5"/>
@@ -6857,17 +7179,17 @@
       <c r="D131" s="6"/>
       <c r="E131" s="6"/>
       <c r="F131" s="5" t="s">
-        <v>797</v>
+        <v>753</v>
       </c>
       <c r="G131" s="5" t="s">
-        <v>994</v>
+        <v>754</v>
       </c>
       <c r="H131" s="5">
-        <v>250</v>
+        <v>1800</v>
       </c>
       <c r="I131" s="5"/>
       <c r="J131" s="4" t="s">
-        <v>992</v>
+        <v>755</v>
       </c>
       <c r="K131" s="4"/>
       <c r="L131" s="4"/>
@@ -6881,28 +7203,24 @@
       <c r="D132" s="6"/>
       <c r="E132" s="6"/>
       <c r="F132" s="5" t="s">
-        <v>106</v>
+        <v>915</v>
       </c>
       <c r="G132" s="5" t="s">
-        <v>23</v>
+        <v>917</v>
       </c>
       <c r="H132" s="5">
-        <v>80</v>
+        <v>400</v>
       </c>
       <c r="I132" s="5"/>
       <c r="J132" s="4" t="s">
-        <v>61</v>
+        <v>916</v>
       </c>
       <c r="K132" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="L132" s="4" t="s">
-        <v>556</v>
-      </c>
+        <v>694</v>
+      </c>
+      <c r="L132" s="4"/>
       <c r="M132" s="4"/>
-      <c r="N132" s="5" t="s">
-        <v>652</v>
-      </c>
+      <c r="N132" s="5"/>
     </row>
     <row r="133" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A133" s="7"/>
@@ -6911,19 +7229,21 @@
       <c r="D133" s="6"/>
       <c r="E133" s="6"/>
       <c r="F133" s="5" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="G133" s="5" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="H133" s="5">
-        <v>350</v>
+        <v>30</v>
       </c>
       <c r="I133" s="5"/>
       <c r="J133" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="K133" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="K133" s="4"/>
       <c r="L133" s="4"/>
       <c r="M133" s="4"/>
       <c r="N133" s="5"/>
@@ -6935,17 +7255,17 @@
       <c r="D134" s="6"/>
       <c r="E134" s="6"/>
       <c r="F134" s="5" t="s">
-        <v>93</v>
+        <v>797</v>
       </c>
       <c r="G134" s="5" t="s">
-        <v>35</v>
+        <v>994</v>
       </c>
       <c r="H134" s="5">
-        <v>400</v>
+        <v>250</v>
       </c>
       <c r="I134" s="5"/>
       <c r="J134" s="4" t="s">
-        <v>62</v>
+        <v>992</v>
       </c>
       <c r="K134" s="4"/>
       <c r="L134" s="4"/>
@@ -6959,18 +7279,28 @@
       <c r="D135" s="6"/>
       <c r="E135" s="6"/>
       <c r="F135" s="5" t="s">
-        <v>749</v>
+        <v>106</v>
       </c>
       <c r="G135" s="5" t="s">
-        <v>798</v>
-      </c>
-      <c r="H135" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="H135" s="5">
+        <v>80</v>
+      </c>
       <c r="I135" s="5"/>
-      <c r="J135" s="4"/>
-      <c r="K135" s="4"/>
-      <c r="L135" s="4"/>
+      <c r="J135" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K135" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="L135" s="4" t="s">
+        <v>556</v>
+      </c>
       <c r="M135" s="4"/>
-      <c r="N135" s="5"/>
+      <c r="N135" s="5" t="s">
+        <v>652</v>
+      </c>
     </row>
     <row r="136" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A136" s="7"/>
@@ -6979,27 +7309,21 @@
       <c r="D136" s="6"/>
       <c r="E136" s="6"/>
       <c r="F136" s="5" t="s">
-        <v>87</v>
+        <v>132</v>
       </c>
       <c r="G136" s="5" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="H136" s="5">
-        <v>60</v>
+        <v>350</v>
       </c>
       <c r="I136" s="5"/>
       <c r="J136" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="K136" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="L136" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="M136" s="4" t="s">
         <v>63</v>
       </c>
+      <c r="K136" s="4"/>
+      <c r="L136" s="4"/>
+      <c r="M136" s="4"/>
       <c r="N136" s="5"/>
     </row>
     <row r="137" spans="1:14" x14ac:dyDescent="0.25">
@@ -7009,17 +7333,17 @@
       <c r="D137" s="6"/>
       <c r="E137" s="6"/>
       <c r="F137" s="5" t="s">
-        <v>205</v>
+        <v>93</v>
       </c>
       <c r="G137" s="5" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="H137" s="5">
-        <v>60</v>
+        <v>400</v>
       </c>
       <c r="I137" s="5"/>
       <c r="J137" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K137" s="4"/>
       <c r="L137" s="4"/>
@@ -7033,21 +7357,15 @@
       <c r="D138" s="6"/>
       <c r="E138" s="6"/>
       <c r="F138" s="5" t="s">
-        <v>669</v>
+        <v>749</v>
       </c>
       <c r="G138" s="5" t="s">
-        <v>637</v>
-      </c>
-      <c r="H138" s="5">
-        <v>60</v>
-      </c>
+        <v>798</v>
+      </c>
+      <c r="H138" s="5"/>
       <c r="I138" s="5"/>
-      <c r="J138" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="K138" s="4" t="s">
-        <v>65</v>
-      </c>
+      <c r="J138" s="4"/>
+      <c r="K138" s="4"/>
       <c r="L138" s="4"/>
       <c r="M138" s="4"/>
       <c r="N138" s="5"/>
@@ -7057,100 +7375,132 @@
       <c r="B139" s="7"/>
       <c r="C139" s="7"/>
       <c r="D139" s="6"/>
-      <c r="E139" s="5"/>
+      <c r="E139" s="6"/>
       <c r="F139" s="5" t="s">
-        <v>805</v>
+        <v>87</v>
       </c>
       <c r="G139" s="5" t="s">
-        <v>803</v>
+        <v>24</v>
       </c>
       <c r="H139" s="5">
-        <v>200</v>
-      </c>
-      <c r="I139" s="5">
-        <v>75</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="I139" s="5"/>
       <c r="J139" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="K139" s="4"/>
-      <c r="L139" s="4"/>
-      <c r="M139" s="4"/>
-      <c r="N139" s="5" t="s">
-        <v>804</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="K139" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="L139" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="M139" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="N139" s="5"/>
     </row>
     <row r="140" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A140" s="5"/>
-      <c r="B140" s="5"/>
+      <c r="A140" s="7"/>
+      <c r="B140" s="7"/>
       <c r="C140" s="7"/>
       <c r="D140" s="6"/>
-      <c r="E140" s="5"/>
+      <c r="E140" s="6"/>
       <c r="F140" s="5" t="s">
-        <v>957</v>
+        <v>205</v>
       </c>
       <c r="G140" s="5" t="s">
-        <v>1022</v>
-      </c>
-      <c r="H140" s="5"/>
+        <v>59</v>
+      </c>
+      <c r="H140" s="5">
+        <v>60</v>
+      </c>
       <c r="I140" s="5"/>
       <c r="J140" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K140" s="4"/>
       <c r="L140" s="4"/>
       <c r="M140" s="4"/>
-      <c r="N140" s="5" t="s">
-        <v>960</v>
-      </c>
+      <c r="N140" s="5"/>
     </row>
     <row r="141" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A141" s="5"/>
-      <c r="B141" s="5"/>
-      <c r="C141" s="5"/>
+      <c r="A141" s="7"/>
+      <c r="B141" s="7"/>
+      <c r="C141" s="7"/>
       <c r="D141" s="6"/>
-      <c r="E141" s="5"/>
-      <c r="F141" s="5"/>
-      <c r="G141" s="5"/>
-      <c r="H141" s="5"/>
+      <c r="E141" s="6"/>
+      <c r="F141" s="5" t="s">
+        <v>669</v>
+      </c>
+      <c r="G141" s="5" t="s">
+        <v>637</v>
+      </c>
+      <c r="H141" s="5">
+        <v>60</v>
+      </c>
       <c r="I141" s="5"/>
-      <c r="J141" s="4"/>
-      <c r="K141" s="4"/>
+      <c r="J141" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="K141" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="L141" s="4"/>
       <c r="M141" s="4"/>
       <c r="N141" s="5"/>
     </row>
     <row r="142" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A142" s="5"/>
-      <c r="B142" s="5"/>
-      <c r="C142" s="5"/>
+      <c r="A142" s="7"/>
+      <c r="B142" s="7"/>
+      <c r="C142" s="7"/>
       <c r="D142" s="6"/>
       <c r="E142" s="5"/>
-      <c r="F142" s="5"/>
-      <c r="G142" s="5"/>
-      <c r="H142" s="5"/>
-      <c r="I142" s="5"/>
-      <c r="J142" s="4"/>
+      <c r="F142" s="5" t="s">
+        <v>805</v>
+      </c>
+      <c r="G142" s="5" t="s">
+        <v>803</v>
+      </c>
+      <c r="H142" s="5">
+        <v>200</v>
+      </c>
+      <c r="I142" s="5">
+        <v>75</v>
+      </c>
+      <c r="J142" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="K142" s="4"/>
       <c r="L142" s="4"/>
       <c r="M142" s="4"/>
-      <c r="N142" s="5"/>
+      <c r="N142" s="5" t="s">
+        <v>804</v>
+      </c>
     </row>
     <row r="143" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A143" s="5"/>
       <c r="B143" s="5"/>
-      <c r="C143" s="5"/>
+      <c r="C143" s="7"/>
       <c r="D143" s="6"/>
       <c r="E143" s="5"/>
-      <c r="F143" s="5"/>
-      <c r="G143" s="5"/>
+      <c r="F143" s="5" t="s">
+        <v>957</v>
+      </c>
+      <c r="G143" s="5" t="s">
+        <v>1022</v>
+      </c>
       <c r="H143" s="5"/>
       <c r="I143" s="5"/>
-      <c r="J143" s="4"/>
+      <c r="J143" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="K143" s="4"/>
       <c r="L143" s="4"/>
       <c r="M143" s="4"/>
-      <c r="N143" s="5"/>
+      <c r="N143" s="5" t="s">
+        <v>960</v>
+      </c>
     </row>
     <row r="144" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A144" s="5"/>
@@ -16241,6 +16591,11 @@
       <c r="N711" s="5"/>
     </row>
     <row r="712" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A712" s="5"/>
+      <c r="B712" s="5"/>
+      <c r="C712" s="5"/>
+      <c r="D712" s="6"/>
+      <c r="E712" s="5"/>
       <c r="F712" s="5"/>
       <c r="G712" s="5"/>
       <c r="H712" s="5"/>
@@ -16252,6 +16607,11 @@
       <c r="N712" s="5"/>
     </row>
     <row r="713" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A713" s="5"/>
+      <c r="B713" s="5"/>
+      <c r="C713" s="5"/>
+      <c r="D713" s="6"/>
+      <c r="E713" s="5"/>
       <c r="F713" s="5"/>
       <c r="G713" s="5"/>
       <c r="H713" s="5"/>
@@ -16263,6 +16623,11 @@
       <c r="N713" s="5"/>
     </row>
     <row r="714" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A714" s="5"/>
+      <c r="B714" s="5"/>
+      <c r="C714" s="5"/>
+      <c r="D714" s="6"/>
+      <c r="E714" s="5"/>
       <c r="F714" s="5"/>
       <c r="G714" s="5"/>
       <c r="H714" s="5"/>
@@ -16327,6 +16692,39 @@
       <c r="L719" s="4"/>
       <c r="M719" s="4"/>
       <c r="N719" s="5"/>
+    </row>
+    <row r="720" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F720" s="5"/>
+      <c r="G720" s="5"/>
+      <c r="H720" s="5"/>
+      <c r="I720" s="5"/>
+      <c r="J720" s="4"/>
+      <c r="K720" s="4"/>
+      <c r="L720" s="4"/>
+      <c r="M720" s="4"/>
+      <c r="N720" s="5"/>
+    </row>
+    <row r="721" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F721" s="5"/>
+      <c r="G721" s="5"/>
+      <c r="H721" s="5"/>
+      <c r="I721" s="5"/>
+      <c r="J721" s="4"/>
+      <c r="K721" s="4"/>
+      <c r="L721" s="4"/>
+      <c r="M721" s="4"/>
+      <c r="N721" s="5"/>
+    </row>
+    <row r="722" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F722" s="5"/>
+      <c r="G722" s="5"/>
+      <c r="H722" s="5"/>
+      <c r="I722" s="5"/>
+      <c r="J722" s="4"/>
+      <c r="K722" s="4"/>
+      <c r="L722" s="4"/>
+      <c r="M722" s="4"/>
+      <c r="N722" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -55319,11 +55717,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L632"/>
+  <dimension ref="A1:L636"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B50" sqref="B50"/>
+      <pane ySplit="2" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D136" sqref="D136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -57575,17 +57973,17 @@
     </row>
     <row r="110" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="7"/>
-      <c r="B110" s="7"/>
+      <c r="B110" s="6"/>
       <c r="C110" s="7"/>
       <c r="D110" s="6"/>
       <c r="E110" s="5" t="s">
-        <v>512</v>
+        <v>1078</v>
       </c>
       <c r="F110" s="5" t="s">
-        <v>330</v>
+        <v>1077</v>
       </c>
       <c r="G110" s="4" t="s">
-        <v>63</v>
+        <v>1076</v>
       </c>
       <c r="H110" s="4"/>
       <c r="I110" s="4"/>
@@ -57599,20 +57997,16 @@
       <c r="C111" s="7"/>
       <c r="D111" s="6"/>
       <c r="E111" s="5" t="s">
-        <v>497</v>
+        <v>512</v>
       </c>
       <c r="F111" s="5" t="s">
-        <v>756</v>
+        <v>330</v>
       </c>
       <c r="G111" s="4" t="s">
-        <v>474</v>
-      </c>
-      <c r="H111" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="I111" s="4" t="s">
         <v>63</v>
       </c>
+      <c r="H111" s="4"/>
+      <c r="I111" s="4"/>
       <c r="J111" s="4"/>
       <c r="K111" s="4"/>
       <c r="L111" s="5"/>
@@ -57623,18 +58017,20 @@
       <c r="C112" s="7"/>
       <c r="D112" s="6"/>
       <c r="E112" s="5" t="s">
-        <v>535</v>
+        <v>497</v>
       </c>
       <c r="F112" s="5" t="s">
-        <v>498</v>
+        <v>756</v>
       </c>
       <c r="G112" s="4" t="s">
         <v>474</v>
       </c>
       <c r="H112" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="I112" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="I112" s="4"/>
       <c r="J112" s="4"/>
       <c r="K112" s="4"/>
       <c r="L112" s="5"/>
@@ -57645,15 +58041,17 @@
       <c r="C113" s="7"/>
       <c r="D113" s="6"/>
       <c r="E113" s="5" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="F113" s="5" t="s">
-        <v>328</v>
+        <v>498</v>
       </c>
       <c r="G113" s="4" t="s">
+        <v>474</v>
+      </c>
+      <c r="H113" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="H113" s="4"/>
       <c r="I113" s="4"/>
       <c r="J113" s="4"/>
       <c r="K113" s="4"/>
@@ -57665,10 +58063,10 @@
       <c r="C114" s="7"/>
       <c r="D114" s="6"/>
       <c r="E114" s="5" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F114" s="5" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="G114" s="4" t="s">
         <v>63</v>
@@ -57681,14 +58079,14 @@
     </row>
     <row r="115" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="7"/>
-      <c r="B115" s="6"/>
+      <c r="B115" s="7"/>
       <c r="C115" s="7"/>
       <c r="D115" s="6"/>
       <c r="E115" s="5" t="s">
-        <v>446</v>
+        <v>537</v>
       </c>
       <c r="F115" s="5" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="G115" s="4" t="s">
         <v>63</v>
@@ -57701,21 +58099,19 @@
     </row>
     <row r="116" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="7"/>
-      <c r="B116" s="7"/>
+      <c r="B116" s="6"/>
       <c r="C116" s="7"/>
       <c r="D116" s="6"/>
       <c r="E116" s="5" t="s">
-        <v>510</v>
+        <v>446</v>
       </c>
       <c r="F116" s="5" t="s">
-        <v>509</v>
+        <v>331</v>
       </c>
       <c r="G116" s="4" t="s">
-        <v>474</v>
-      </c>
-      <c r="H116" s="4" t="s">
         <v>63</v>
       </c>
+      <c r="H116" s="4"/>
       <c r="I116" s="4"/>
       <c r="J116" s="4"/>
       <c r="K116" s="4"/>
@@ -57727,13 +58123,13 @@
       <c r="C117" s="7"/>
       <c r="D117" s="6"/>
       <c r="E117" s="5" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F117" s="5" t="s">
-        <v>631</v>
+        <v>509</v>
       </c>
       <c r="G117" s="4" t="s">
-        <v>68</v>
+        <v>474</v>
       </c>
       <c r="H117" s="4" t="s">
         <v>63</v>
@@ -57747,17 +58143,19 @@
       <c r="A118" s="7"/>
       <c r="B118" s="7"/>
       <c r="C118" s="7"/>
-      <c r="D118" s="7"/>
+      <c r="D118" s="6"/>
       <c r="E118" s="5" t="s">
-        <v>551</v>
+        <v>511</v>
       </c>
       <c r="F118" s="5" t="s">
-        <v>550</v>
+        <v>631</v>
       </c>
       <c r="G118" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="H118" s="4"/>
+      <c r="H118" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="I118" s="4"/>
       <c r="J118" s="4"/>
       <c r="K118" s="4"/>
@@ -57766,20 +58164,18 @@
     <row r="119" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="7"/>
       <c r="B119" s="7"/>
-      <c r="C119" s="17"/>
-      <c r="D119" s="6"/>
+      <c r="C119" s="7"/>
+      <c r="D119" s="7"/>
       <c r="E119" s="5" t="s">
-        <v>910</v>
+        <v>551</v>
       </c>
       <c r="F119" s="5" t="s">
-        <v>909</v>
+        <v>550</v>
       </c>
       <c r="G119" s="4" t="s">
-        <v>694</v>
-      </c>
-      <c r="H119" s="4" t="s">
-        <v>66</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="H119" s="4"/>
       <c r="I119" s="4"/>
       <c r="J119" s="4"/>
       <c r="K119" s="4"/>
@@ -57788,18 +58184,20 @@
     <row r="120" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="7"/>
       <c r="B120" s="7"/>
-      <c r="C120" s="7"/>
+      <c r="C120" s="17"/>
       <c r="D120" s="6"/>
       <c r="E120" s="5" t="s">
-        <v>557</v>
+        <v>910</v>
       </c>
       <c r="F120" s="5" t="s">
-        <v>333</v>
+        <v>909</v>
       </c>
       <c r="G120" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="H120" s="4"/>
+        <v>694</v>
+      </c>
+      <c r="H120" s="4" t="s">
+        <v>66</v>
+      </c>
       <c r="I120" s="4"/>
       <c r="J120" s="4"/>
       <c r="K120" s="4"/>
@@ -57811,10 +58209,10 @@
       <c r="C121" s="7"/>
       <c r="D121" s="6"/>
       <c r="E121" s="5" t="s">
-        <v>468</v>
+        <v>557</v>
       </c>
       <c r="F121" s="5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G121" s="4" t="s">
         <v>63</v>
@@ -57828,20 +58226,18 @@
     <row r="122" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="7"/>
       <c r="B122" s="7"/>
-      <c r="C122" s="17"/>
+      <c r="C122" s="7"/>
       <c r="D122" s="6"/>
       <c r="E122" s="5" t="s">
-        <v>908</v>
+        <v>468</v>
       </c>
       <c r="F122" s="5" t="s">
-        <v>907</v>
+        <v>334</v>
       </c>
       <c r="G122" s="4" t="s">
-        <v>694</v>
-      </c>
-      <c r="H122" s="4" t="s">
-        <v>66</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="H122" s="4"/>
       <c r="I122" s="4"/>
       <c r="J122" s="4"/>
       <c r="K122" s="4"/>
@@ -57850,18 +58246,20 @@
     <row r="123" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="7"/>
       <c r="B123" s="7"/>
-      <c r="C123" s="7"/>
+      <c r="C123" s="17"/>
       <c r="D123" s="6"/>
       <c r="E123" s="5" t="s">
-        <v>545</v>
+        <v>908</v>
       </c>
       <c r="F123" s="5" t="s">
-        <v>358</v>
+        <v>907</v>
       </c>
       <c r="G123" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="H123" s="4"/>
+        <v>694</v>
+      </c>
+      <c r="H123" s="4" t="s">
+        <v>66</v>
+      </c>
       <c r="I123" s="4"/>
       <c r="J123" s="4"/>
       <c r="K123" s="4"/>
@@ -57873,13 +58271,13 @@
       <c r="C124" s="7"/>
       <c r="D124" s="6"/>
       <c r="E124" s="5" t="s">
-        <v>540</v>
+        <v>545</v>
       </c>
       <c r="F124" s="5" t="s">
-        <v>332</v>
+        <v>358</v>
       </c>
       <c r="G124" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H124" s="4"/>
       <c r="I124" s="4"/>
@@ -57893,13 +58291,13 @@
       <c r="C125" s="7"/>
       <c r="D125" s="6"/>
       <c r="E125" s="5" t="s">
-        <v>447</v>
+        <v>540</v>
       </c>
       <c r="F125" s="5" t="s">
-        <v>305</v>
+        <v>332</v>
       </c>
       <c r="G125" s="4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H125" s="4"/>
       <c r="I125" s="4"/>
@@ -57913,13 +58311,13 @@
       <c r="C126" s="7"/>
       <c r="D126" s="6"/>
       <c r="E126" s="5" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="F126" s="5" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="G126" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H126" s="4"/>
       <c r="I126" s="4"/>
@@ -57933,13 +58331,13 @@
       <c r="C127" s="7"/>
       <c r="D127" s="6"/>
       <c r="E127" s="5" t="s">
-        <v>467</v>
+        <v>452</v>
       </c>
       <c r="F127" s="5" t="s">
-        <v>326</v>
+        <v>310</v>
       </c>
       <c r="G127" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H127" s="4"/>
       <c r="I127" s="4"/>
@@ -57953,13 +58351,13 @@
       <c r="C128" s="7"/>
       <c r="D128" s="6"/>
       <c r="E128" s="5" t="s">
-        <v>448</v>
+        <v>467</v>
       </c>
       <c r="F128" s="5" t="s">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="G128" s="4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H128" s="4"/>
       <c r="I128" s="4"/>
@@ -57973,13 +58371,13 @@
       <c r="C129" s="7"/>
       <c r="D129" s="6"/>
       <c r="E129" s="5" t="s">
-        <v>466</v>
+        <v>448</v>
       </c>
       <c r="F129" s="5" t="s">
-        <v>325</v>
+        <v>306</v>
       </c>
       <c r="G129" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H129" s="4"/>
       <c r="I129" s="4"/>
@@ -57989,17 +58387,17 @@
     </row>
     <row r="130" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="7"/>
-      <c r="B130" s="7"/>
+      <c r="B130" s="6"/>
       <c r="C130" s="7"/>
       <c r="D130" s="6"/>
       <c r="E130" s="5" t="s">
-        <v>465</v>
+        <v>1030</v>
       </c>
       <c r="F130" s="5" t="s">
-        <v>324</v>
+        <v>1029</v>
       </c>
       <c r="G130" s="4" t="s">
-        <v>63</v>
+        <v>825</v>
       </c>
       <c r="H130" s="4"/>
       <c r="I130" s="4"/>
@@ -58013,10 +58411,10 @@
       <c r="C131" s="7"/>
       <c r="D131" s="6"/>
       <c r="E131" s="5" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="F131" s="5" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="G131" s="4" t="s">
         <v>63</v>
@@ -58027,16 +58425,16 @@
       <c r="K131" s="4"/>
       <c r="L131" s="5"/>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="7"/>
       <c r="B132" s="7"/>
       <c r="C132" s="7"/>
       <c r="D132" s="6"/>
       <c r="E132" s="5" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="F132" s="5" t="s">
-        <v>347</v>
+        <v>324</v>
       </c>
       <c r="G132" s="4" t="s">
         <v>63</v>
@@ -58047,16 +58445,16 @@
       <c r="K132" s="4"/>
       <c r="L132" s="5"/>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="7"/>
       <c r="B133" s="7"/>
       <c r="C133" s="7"/>
       <c r="D133" s="6"/>
       <c r="E133" s="5" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="F133" s="5" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="G133" s="4" t="s">
         <v>63</v>
@@ -58073,13 +58471,13 @@
       <c r="C134" s="7"/>
       <c r="D134" s="6"/>
       <c r="E134" s="5" t="s">
-        <v>434</v>
+        <v>472</v>
       </c>
       <c r="F134" s="5" t="s">
-        <v>273</v>
+        <v>347</v>
       </c>
       <c r="G134" s="4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H134" s="4"/>
       <c r="I134" s="4"/>
@@ -58093,13 +58491,13 @@
       <c r="C135" s="7"/>
       <c r="D135" s="6"/>
       <c r="E135" s="5" t="s">
-        <v>433</v>
+        <v>463</v>
       </c>
       <c r="F135" s="5" t="s">
-        <v>359</v>
+        <v>322</v>
       </c>
       <c r="G135" s="4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H135" s="4"/>
       <c r="I135" s="4"/>
@@ -58107,19 +58505,19 @@
       <c r="K135" s="4"/>
       <c r="L135" s="5"/>
     </row>
-    <row r="136" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A136" s="7"/>
       <c r="B136" s="7"/>
       <c r="C136" s="7"/>
       <c r="D136" s="6"/>
       <c r="E136" s="5" t="s">
-        <v>786</v>
+        <v>434</v>
       </c>
       <c r="F136" s="5" t="s">
-        <v>785</v>
+        <v>273</v>
       </c>
       <c r="G136" s="4" t="s">
-        <v>694</v>
+        <v>61</v>
       </c>
       <c r="H136" s="4"/>
       <c r="I136" s="4"/>
@@ -58129,17 +58527,17 @@
     </row>
     <row r="137" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A137" s="7"/>
-      <c r="B137" s="7"/>
+      <c r="B137" s="6"/>
       <c r="C137" s="7"/>
       <c r="D137" s="6"/>
       <c r="E137" s="5" t="s">
-        <v>819</v>
+        <v>1032</v>
       </c>
       <c r="F137" s="5" t="s">
-        <v>818</v>
+        <v>1031</v>
       </c>
       <c r="G137" s="4" t="s">
-        <v>63</v>
+        <v>694</v>
       </c>
       <c r="H137" s="4"/>
       <c r="I137" s="4"/>
@@ -58149,17 +58547,17 @@
     </row>
     <row r="138" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A138" s="7"/>
-      <c r="B138" s="7"/>
+      <c r="B138" s="6"/>
       <c r="C138" s="7"/>
       <c r="D138" s="6"/>
       <c r="E138" s="5" t="s">
-        <v>821</v>
+        <v>1079</v>
       </c>
       <c r="F138" s="5" t="s">
-        <v>820</v>
+        <v>1080</v>
       </c>
       <c r="G138" s="4" t="s">
-        <v>63</v>
+        <v>1076</v>
       </c>
       <c r="H138" s="4"/>
       <c r="I138" s="4"/>
@@ -58173,13 +58571,13 @@
       <c r="C139" s="7"/>
       <c r="D139" s="6"/>
       <c r="E139" s="5" t="s">
-        <v>823</v>
+        <v>433</v>
       </c>
       <c r="F139" s="5" t="s">
-        <v>822</v>
+        <v>359</v>
       </c>
       <c r="G139" s="4" t="s">
-        <v>694</v>
+        <v>61</v>
       </c>
       <c r="H139" s="4"/>
       <c r="I139" s="4"/>
@@ -58187,19 +58585,19 @@
       <c r="K139" s="4"/>
       <c r="L139" s="5"/>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="7"/>
       <c r="B140" s="7"/>
       <c r="C140" s="7"/>
       <c r="D140" s="6"/>
       <c r="E140" s="5" t="s">
-        <v>826</v>
+        <v>786</v>
       </c>
       <c r="F140" s="5" t="s">
-        <v>824</v>
+        <v>785</v>
       </c>
       <c r="G140" s="4" t="s">
-        <v>825</v>
+        <v>694</v>
       </c>
       <c r="H140" s="4"/>
       <c r="I140" s="4"/>
@@ -58213,13 +58611,13 @@
       <c r="C141" s="7"/>
       <c r="D141" s="6"/>
       <c r="E141" s="5" t="s">
-        <v>855</v>
+        <v>819</v>
       </c>
       <c r="F141" s="5" t="s">
-        <v>854</v>
+        <v>818</v>
       </c>
       <c r="G141" s="4" t="s">
-        <v>755</v>
+        <v>63</v>
       </c>
       <c r="H141" s="4"/>
       <c r="I141" s="4"/>
@@ -58233,13 +58631,13 @@
       <c r="C142" s="7"/>
       <c r="D142" s="6"/>
       <c r="E142" s="5" t="s">
-        <v>867</v>
+        <v>821</v>
       </c>
       <c r="F142" s="5" t="s">
-        <v>865</v>
+        <v>820</v>
       </c>
       <c r="G142" s="4" t="s">
-        <v>866</v>
+        <v>63</v>
       </c>
       <c r="H142" s="4"/>
       <c r="I142" s="4"/>
@@ -58248,40 +58646,38 @@
       <c r="L142" s="5"/>
     </row>
     <row r="143" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A143" s="17"/>
-      <c r="B143" s="6"/>
-      <c r="C143" s="17"/>
+      <c r="A143" s="7"/>
+      <c r="B143" s="7"/>
+      <c r="C143" s="7"/>
       <c r="D143" s="6"/>
       <c r="E143" s="5" t="s">
-        <v>966</v>
+        <v>823</v>
       </c>
       <c r="F143" s="5" t="s">
-        <v>964</v>
+        <v>822</v>
       </c>
       <c r="G143" s="4" t="s">
-        <v>65</v>
+        <v>694</v>
       </c>
       <c r="H143" s="4"/>
       <c r="I143" s="4"/>
       <c r="J143" s="4"/>
       <c r="K143" s="4"/>
-      <c r="L143" s="5" t="s">
-        <v>965</v>
-      </c>
+      <c r="L143" s="5"/>
     </row>
     <row r="144" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A144" s="17"/>
+      <c r="A144" s="7"/>
       <c r="B144" s="7"/>
-      <c r="C144" s="17"/>
+      <c r="C144" s="7"/>
       <c r="D144" s="6"/>
       <c r="E144" s="5" t="s">
-        <v>968</v>
+        <v>826</v>
       </c>
       <c r="F144" s="5" t="s">
-        <v>967</v>
+        <v>824</v>
       </c>
       <c r="G144" s="4" t="s">
-        <v>65</v>
+        <v>825</v>
       </c>
       <c r="H144" s="4"/>
       <c r="I144" s="4"/>
@@ -58295,13 +58691,13 @@
       <c r="C145" s="7"/>
       <c r="D145" s="6"/>
       <c r="E145" s="5" t="s">
-        <v>970</v>
+        <v>855</v>
       </c>
       <c r="F145" s="5" t="s">
-        <v>969</v>
+        <v>854</v>
       </c>
       <c r="G145" s="4" t="s">
-        <v>63</v>
+        <v>755</v>
       </c>
       <c r="H145" s="4"/>
       <c r="I145" s="4"/>
@@ -58311,17 +58707,17 @@
     </row>
     <row r="146" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A146" s="7"/>
-      <c r="B146" s="6"/>
+      <c r="B146" s="7"/>
       <c r="C146" s="7"/>
       <c r="D146" s="6"/>
       <c r="E146" s="5" t="s">
-        <v>972</v>
+        <v>867</v>
       </c>
       <c r="F146" s="5" t="s">
-        <v>971</v>
+        <v>865</v>
       </c>
       <c r="G146" s="4" t="s">
-        <v>63</v>
+        <v>866</v>
       </c>
       <c r="H146" s="4"/>
       <c r="I146" s="4"/>
@@ -58330,27 +58726,41 @@
       <c r="L146" s="5"/>
     </row>
     <row r="147" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A147" s="6"/>
+      <c r="A147" s="17"/>
       <c r="B147" s="6"/>
-      <c r="C147" s="6"/>
+      <c r="C147" s="17"/>
       <c r="D147" s="6"/>
-      <c r="E147" s="5"/>
-      <c r="F147" s="5"/>
-      <c r="G147" s="4"/>
+      <c r="E147" s="5" t="s">
+        <v>966</v>
+      </c>
+      <c r="F147" s="5" t="s">
+        <v>964</v>
+      </c>
+      <c r="G147" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="H147" s="4"/>
       <c r="I147" s="4"/>
       <c r="J147" s="4"/>
       <c r="K147" s="4"/>
-      <c r="L147" s="5"/>
+      <c r="L147" s="5" t="s">
+        <v>965</v>
+      </c>
     </row>
     <row r="148" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A148" s="6"/>
-      <c r="B148" s="6"/>
-      <c r="C148" s="6"/>
+      <c r="A148" s="17"/>
+      <c r="B148" s="7"/>
+      <c r="C148" s="17"/>
       <c r="D148" s="6"/>
-      <c r="E148" s="5"/>
-      <c r="F148" s="5"/>
-      <c r="G148" s="4"/>
+      <c r="E148" s="5" t="s">
+        <v>968</v>
+      </c>
+      <c r="F148" s="5" t="s">
+        <v>967</v>
+      </c>
+      <c r="G148" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="H148" s="4"/>
       <c r="I148" s="4"/>
       <c r="J148" s="4"/>
@@ -58358,13 +58768,19 @@
       <c r="L148" s="5"/>
     </row>
     <row r="149" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A149" s="6"/>
-      <c r="B149" s="6"/>
-      <c r="C149" s="6"/>
+      <c r="A149" s="7"/>
+      <c r="B149" s="7"/>
+      <c r="C149" s="7"/>
       <c r="D149" s="6"/>
-      <c r="E149" s="5"/>
-      <c r="F149" s="5"/>
-      <c r="G149" s="4"/>
+      <c r="E149" s="5" t="s">
+        <v>970</v>
+      </c>
+      <c r="F149" s="5" t="s">
+        <v>969</v>
+      </c>
+      <c r="G149" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="H149" s="4"/>
       <c r="I149" s="4"/>
       <c r="J149" s="4"/>
@@ -58372,13 +58788,19 @@
       <c r="L149" s="5"/>
     </row>
     <row r="150" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A150" s="6"/>
+      <c r="A150" s="7"/>
       <c r="B150" s="6"/>
-      <c r="C150" s="6"/>
+      <c r="C150" s="7"/>
       <c r="D150" s="6"/>
-      <c r="E150" s="5"/>
-      <c r="F150" s="5"/>
-      <c r="G150" s="4"/>
+      <c r="E150" s="5" t="s">
+        <v>972</v>
+      </c>
+      <c r="F150" s="5" t="s">
+        <v>971</v>
+      </c>
+      <c r="G150" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="H150" s="4"/>
       <c r="I150" s="4"/>
       <c r="J150" s="4"/>
@@ -58974,10 +59396,10 @@
       <c r="L192" s="5"/>
     </row>
     <row r="193" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A193" s="5"/>
-      <c r="B193" s="5"/>
-      <c r="C193" s="5"/>
-      <c r="D193" s="5"/>
+      <c r="A193" s="6"/>
+      <c r="B193" s="6"/>
+      <c r="C193" s="6"/>
+      <c r="D193" s="6"/>
       <c r="E193" s="5"/>
       <c r="F193" s="5"/>
       <c r="G193" s="4"/>
@@ -58988,10 +59410,10 @@
       <c r="L193" s="5"/>
     </row>
     <row r="194" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A194" s="5"/>
-      <c r="B194" s="5"/>
-      <c r="C194" s="5"/>
-      <c r="D194" s="5"/>
+      <c r="A194" s="6"/>
+      <c r="B194" s="6"/>
+      <c r="C194" s="6"/>
+      <c r="D194" s="6"/>
       <c r="E194" s="5"/>
       <c r="F194" s="5"/>
       <c r="G194" s="4"/>
@@ -59002,10 +59424,10 @@
       <c r="L194" s="5"/>
     </row>
     <row r="195" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A195" s="5"/>
-      <c r="B195" s="5"/>
-      <c r="C195" s="5"/>
-      <c r="D195" s="5"/>
+      <c r="A195" s="6"/>
+      <c r="B195" s="6"/>
+      <c r="C195" s="6"/>
+      <c r="D195" s="6"/>
       <c r="E195" s="5"/>
       <c r="F195" s="5"/>
       <c r="G195" s="4"/>
@@ -59016,10 +59438,10 @@
       <c r="L195" s="5"/>
     </row>
     <row r="196" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A196" s="5"/>
-      <c r="B196" s="5"/>
-      <c r="C196" s="5"/>
-      <c r="D196" s="5"/>
+      <c r="A196" s="6"/>
+      <c r="B196" s="6"/>
+      <c r="C196" s="6"/>
+      <c r="D196" s="6"/>
       <c r="E196" s="5"/>
       <c r="F196" s="5"/>
       <c r="G196" s="4"/>
@@ -65133,6 +65555,62 @@
       <c r="K632" s="4"/>
       <c r="L632" s="5"/>
     </row>
+    <row r="633" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A633" s="5"/>
+      <c r="B633" s="5"/>
+      <c r="C633" s="5"/>
+      <c r="D633" s="5"/>
+      <c r="E633" s="5"/>
+      <c r="F633" s="5"/>
+      <c r="G633" s="4"/>
+      <c r="H633" s="4"/>
+      <c r="I633" s="4"/>
+      <c r="J633" s="4"/>
+      <c r="K633" s="4"/>
+      <c r="L633" s="5"/>
+    </row>
+    <row r="634" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A634" s="5"/>
+      <c r="B634" s="5"/>
+      <c r="C634" s="5"/>
+      <c r="D634" s="5"/>
+      <c r="E634" s="5"/>
+      <c r="F634" s="5"/>
+      <c r="G634" s="4"/>
+      <c r="H634" s="4"/>
+      <c r="I634" s="4"/>
+      <c r="J634" s="4"/>
+      <c r="K634" s="4"/>
+      <c r="L634" s="5"/>
+    </row>
+    <row r="635" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A635" s="5"/>
+      <c r="B635" s="5"/>
+      <c r="C635" s="5"/>
+      <c r="D635" s="5"/>
+      <c r="E635" s="5"/>
+      <c r="F635" s="5"/>
+      <c r="G635" s="4"/>
+      <c r="H635" s="4"/>
+      <c r="I635" s="4"/>
+      <c r="J635" s="4"/>
+      <c r="K635" s="4"/>
+      <c r="L635" s="5"/>
+    </row>
+    <row r="636" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A636" s="5"/>
+      <c r="B636" s="5"/>
+      <c r="C636" s="5"/>
+      <c r="D636" s="5"/>
+      <c r="E636" s="5"/>
+      <c r="F636" s="5"/>
+      <c r="G636" s="4"/>
+      <c r="H636" s="4"/>
+      <c r="I636" s="4"/>
+      <c r="J636" s="4"/>
+      <c r="K636" s="4"/>
+      <c r="L636" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -65144,7 +65622,7 @@
   <dimension ref="A1:B409"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -68428,4 +68906,520 @@
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D44"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.85546875" style="21" customWidth="1"/>
+    <col min="2" max="3" width="6.5703125" style="15" customWidth="1"/>
+    <col min="4" max="4" width="68.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="25" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>1033</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>1034</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="18" t="s">
+        <v>1070</v>
+      </c>
+      <c r="D4" s="6"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
+        <v>752</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
+        <v>555</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="22">
+        <v>0.95</v>
+      </c>
+      <c r="D9" s="6"/>
+    </row>
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
+        <v>1081</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="22">
+        <v>0.99</v>
+      </c>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="20" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="20" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="6"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="20" t="s">
+        <v>914</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="6"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="20" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="20" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="22">
+        <v>0.9</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="20" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="20" t="s">
+        <v>474</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="6"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="20" t="s">
+        <v>866</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="22">
+        <v>0.75</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="20" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="6"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="20" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="22">
+        <v>0.98</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="20" t="s">
+        <v>992</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="6" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="6" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="20" t="s">
+        <v>916</v>
+      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="6"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="20" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="20" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B26" s="7"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="20" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B27" s="6"/>
+      <c r="C27" s="22">
+        <v>0.9</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="20" t="s">
+        <v>974</v>
+      </c>
+      <c r="B28" s="6"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="6" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="20" t="s">
+        <v>755</v>
+      </c>
+      <c r="B29" s="7"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="20" t="s">
+        <v>417</v>
+      </c>
+      <c r="B30" s="6"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="6"/>
+    </row>
+    <row r="31" spans="1:4" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D31" s="15"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="23" t="s">
+        <v>1059</v>
+      </c>
+      <c r="B32" s="24" t="s">
+        <v>1033</v>
+      </c>
+      <c r="C32" s="24" t="s">
+        <v>1034</v>
+      </c>
+      <c r="D32" s="24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="20" t="s">
+        <v>690</v>
+      </c>
+      <c r="B33" s="6"/>
+      <c r="C33" s="22">
+        <v>0.75</v>
+      </c>
+      <c r="D33" s="6"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="20" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B34" s="6"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="6" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="20" t="s">
+        <v>751</v>
+      </c>
+      <c r="B35" s="7"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="20" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B36" s="6"/>
+      <c r="C36" s="22">
+        <v>0.95</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>1058</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="20" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B37" s="6"/>
+      <c r="C37" s="32"/>
+      <c r="D37" s="6" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="20" t="s">
+        <v>1084</v>
+      </c>
+      <c r="B38" s="7"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="20" t="s">
+        <v>1082</v>
+      </c>
+      <c r="B39" s="7"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="20" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B40" s="7"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="20" t="s">
+        <v>749</v>
+      </c>
+      <c r="B41" s="7"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+    </row>
+    <row r="42" spans="1:4" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="23" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B43" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" s="27"/>
+      <c r="D43" s="28"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="20" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B44" s="29" t="s">
+        <v>1063</v>
+      </c>
+      <c r="C44" s="30"/>
+      <c r="D44" s="31"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B44:D44"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1096</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>